<commit_message>
Implemented travel time and distance
</commit_message>
<xml_diff>
--- a/Indeed_WebScrape/jobsDf.xlsx
+++ b/Indeed_WebScrape/jobsDf.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,37 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Short Description</t>
+          <t>Easy_Apply</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Contract_Type</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Distance</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Travel_Time</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Short_Description</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Full_Description</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
         </is>
       </c>
     </row>
@@ -461,12 +491,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Data Scientist</t>
+          <t>Sr. Data Scientist (Remote)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Business Science</t>
+          <t>CrowdStrike</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -474,10 +504,63 @@
           <t>United Kingdom•Remote</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>4-6 years’ experience in a technical / data scientist role.
-Address business challenges by leveraging analytics and data science to provide meaningful and…</t>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Have experience working on very large data sets of sparse high dimensional data and experience in pre-processing and analyzing such data to gain actionable…</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>At CrowdStrike we’re on a mission - to stop breaches. Our groundbreaking technology, services delivery, and intelligence gathering together with our innovations in machine learning and behavioral-based detection, allow our customers to not only defend themselves, but do so in a future-proof manner. We’ve earned numerous honors and top rankings for our technology, organization and people – clearly confirming our industry leadership and our special culture driving it. We also offer flexible work arrangements to help our people manage their personal and professional lives in a way that works for them. So if you’re ready to work on unrivaled technology where your desire to be part of a collaborative team is met with a laser-focused mission to stop breaches and protect people globally, let’s talk.
+About the Role:
+CrowdStrike EndPoint Protection team is expanding. We are looking for data scientists to help us build solutions with detections based on indicators of risk, analytics and risk scoring. You will have the opportunity to apply your coding, mathematical and scientific research skills to the bleeding edge of security technology. You’ll be able to leverage large-scale rich data to meaningfully improve our supervised learning models and refine our identification of malicious computer software and behavioral threats. CrowdStrike’s cybersecurity data is one-of-a-kind: we process over 1 trillion behavioral events per day and have over 2000 terabytes of malware samples in our research repository. We are a diverse and multidisciplinary team, and you’ll have the chance to broaden your horizons by working jointly with a team of Big Data, Machine Learning, and Security domain experts on hard and impactful problems.
+What You'll Need:
+Undergraduate or postgraduate degree in a STEM field
+Extensive post/undergraduate experience in data science, machine learning, or any field employing computational science or data driven analyses
+Programming experience in Python or Scala
+You will:
+Mine large scale and high dimensional data, identify patterns, and visualize trends
+Create predictive models using supervised learning techniques to detect and stop the most sophisticated threats
+Innovate new semi-supervised and online learning techniques to enhance our threat detection capabilities and reduce nuisance false positives for our customers.
+Work closely with domain experts to improve our raw data and to derive more value from data collected
+Hone your ability to balance detail-oriented research with goal-oriented business objectives
+Implement and experiment with new algorithms and methodologies to help improve our machine learning models
+Automate and visualize analyses, results and processes in our machine learning pipeline
+You are:
+Passionate about cybersecurity, with a firm understanding of the problem space or passionate about applying your machine learning skillset to new domain areas such as cybersecurity
+Versed in utilizing Machine Learning techniques and familiar with the standard algorithms, their trade-offs, their usage, and how to tune them
+Have experience working on very large data sets of sparse high dimensional data and experience in pre-processing and analyzing such data to gain actionable insights
+An independent self-starter who likes to take ownership and independently seeks out new challenges
+Thirsty for knowledge and do not hesitate to step outside of your comfort zone to learn new technologies, algorithms and concepts
+Comfortable to dive into a Python codebase, including experience with unit testing and the python packaging ecosystem
+Comfortable and experienced working in a Linux environment in the AWS cloud
+Analytically minded: never afraid to drill down into a data-set, or debug-deeper into an unfamiliar codebase
+#LI-MC1
+#LI-Remote
+Benefits of Working at CrowdStrike:
+Market leader in compensation and equity awards
+Competitive vacation policy
+Comprehensive health benefits
+Flexible work environment
+Wellness programs
+Stocked fridges, coffee, soda, and lots of treats
+We are committed to building an inclusive culture of belonging that not only embraces the diversity of our people but also reflects the diversity of the communities in which we work and the customers we serve. We know that the happiest and highest performing teams include people with diverse perspectives and ways of solving problems so we strive to attract and retain talent from all backgrounds and create workplaces where everyone feels empowered to bring their full, authentic selves to work.
+CrowdStrike is an Equal Opportunity employer. All qualified applicants will receive consideration for employment without regard to race, color, religion, sex including sexual orientation and gender identity, national origin, disability, protected veteran status, or any other characteristic protected by applicable federal, state, or local law.</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0BJMW_X9OCLkZ04_weh8WkR-IGNb1MhigwTP7XGwrJOF_X_VSZLnRc8x9p7EGl99QfnO7rcpARi_jZFAi1DQHRR86_6bF7GzryOxmNFcCt0jbPYDtl2FnYUy7DwD_4SPcZwsD3f4vyYqLRca812fYP7F8n8_9C7erjuqEi08KoOkZEWVoCL6ai9QF3kCu8rhr_ShSOywtbPRt4zaE8GaodWl1-xjz9b5wIOozBirZ7HqTDfPDi7pYZFyYc0FId_otSUUkyVYr1cyfufrqZ7yMHchJ3YXZoWbYYgAx6_NHuBaUQ8uA4Bbj_57GjLTgwojtROjLSSfrrN4ciZ24qAbkb4RU23x6_vs9227DGA_ZiHD3gURO6zjohAXaDDquJHmNn8OraSx4m9Kt0Wgb_YN5reMY9wgDVHBJJIvzyzhyQM0CKWGg3UCLAGPiIupJRWa9CL0LOgxIWs0zdD5UtTQaLuwGkmrL4Y2YAAgq8O-yocvVAEie4PCy6ccYf-_btGfToUYsSIMT_DcVtRcM3lnE9l0OgTk9wMgEnxlvdHv9jVeOhmUpP4wrXo&amp;p=0&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -487,23 +570,60 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Data Scientist</t>
+          <t>Defence Data Scientist</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Moonpig</t>
+          <t>Metrica Recruitment</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Excellent skills within either Python or R and SQL skills (so you can self-serve your own data).
-This means that no matter which function a project is for, you…</t>
+          <t>South West</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>£40,000 - £45,000 a year</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>167.4113</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2:20:06</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Three years' or more of experience in data science.
+Your role would be to develop and design decision aid tools and models to carry out analysis for customers…</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>The Company
+This highly successful strategy consultancy specialise in the government and defence sectors.
+They have significant innovation funding from the MoD, meaning that they don't just pitch an idea to improve what's in place but actually have to prove that something has never been done before and is genuinely different to anything or anyone else.
+The Role
+Your role would be to develop and design decision aid tools and models to carry out analysis for customers and more recently, there has been an increased focus on product development. The content of decision aids, used for strategic or operational decision making, is predominantly AI based machine learning and there are a range of unique techniques developed internally.
+A niche but exciting area they work in is explainable AI, which is a part of past, current projects and future plans. Given that clients are typically within the defence sector, when machine learning algorithms spit out an answer, it's not possible to simply rely on the computer saying this is what you should do. It's essential to add reasons why, which is challenging to generate from standard ML algorithms.
+The Individual
+Three years' or more of experience in data science.
+Strong Python proficiency.
+Excellent communication skills, both verbal and written.
+To acquire security clearance, it's a necessity that you have lived in the UK for five consecutive years without spending more than three consecutive months out of the UK.
+Job Owner: d.prosser</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0B4I0z8Vg4C22bXJk453pUE2nnLCUOyY_R-ihB16RDW65dAXO9w17QY8SOm2HP94HptMLXv5tQJz9tiF4ev5eCB4EYCTHe-YzBJKwMAnjDabRN056LgA49BqFgm_-BvDdVh6acr-5rEEdCObYarf9kGPomUSuya6N7oGNCnjHCdq9tr4EL2gSBmLJVWksWww70M6mRt-8ofZNSeK88XLYo70iucoBUsTk7ten_BnhCwp-5VRI35IL30_VeyFxJCYZKdoP_eXYl_kV6h8td3TOJKlxHT02CYMUp1BZVu5T4SvsV4i1aoJ1yoRAOwdfA-pnVpiEum2s4kG0Q_Pvnmr8DdG1DWtlKxDsTi_JwGfNBxq2DG3UeGtKv--EILNyxnRqeGqsARsahpMpvkBKh4AlmRco_16hSvNz298hE8C_0iigU7LBYbzZvpxydY0ZUtSmg1F_N3DqqLabb6HT-1yjCoxKcO5Kup1YXP3YyoTTxrM3gBQlWrRM1O6Z-N7MGIyhgs6AvCIXU0YMfe6rMG3S349bxA6W-9JjTP2IJrPbNE4lyPZD8vmEhR5i6Kj52WF7iubM5AzYUPShWPaiGf9qzoHAxi83K4QvjNk2jHJ8h1OQPQe1EDqLmPKr_Wo3cTvyooN77J1PGn2vZdYXNIKyDu7lrtxBPO0V8tIOUZeFMjqmd8AIBIw0iePRz_MfOrmFk=&amp;p=1&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -513,23 +633,81 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Defence Data Scientist</t>
+          <t>Modernization Data Scientist/Visualization - VP</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Metrica Recruitment</t>
+          <t>JPMorgan Chase Bank, N.A.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>South West</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Three years' or more of experience in data science.
-Your role would be to develop and design decision aid tools and models to carry out analysis for customers…</t>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Full-time, Permanent</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>9.039200000000001</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0:14:30</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Modify and blend data by designing workflows in the Alteryx application to harvest, validate, clean and standardize data in a highly repeatable manner.</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>This position will be a Tableau &amp; Alteryx Dashboard Developer for the Corporate Technology Office (CTO) dashboards, which will directly report to the CTO Portfolio Insights Product Owner and will partner closely with the CTO Modernization Execution leads. The remit will encompass all end to end requirements to prioritization, planning and execution of work inclusive of infrastructure design, test execution, and implementation. The successful candidate must possess strong analytical &amp; problem-solving skills, have the ability to prioritize and manage time.
+KEY RESPONSIBILITIES:
+Develop dynamic, scalable and effective dashboards in Tableau using Alteryx and other data wrangling tools to summarize and analyze key business drivers using Safe, LEAN, Agile methodologies
+Leverage a strong foundational knowledge of financial, application and developer metrics to build effective solutions that simplify, automate, and add value
+Create robust and stable data pipelines as well as efficient data maps for optimal Tableau performance
+Express creativity and ingenuity to transform how we see and understand data
+Perform data integration, write efficient SQL Queries, and develop/deploy reporting solutions that apply data visualization standards and best practices, and meets quality standards by performing unit testing
+Query with SQL or Python scrips, configure APIs used to connect data sources.
+Modify and blend data by designing workflows in the Alteryx application to harvest, validate, clean and standardize data in a highly repeatable manner
+Understand the variety of sources for information and how to strategically source data
+Tracking development and deployment timelines
+User Acceptance Testing and Validation of new dashboards
+Gather, interpret and analyze business requirements and use cases and design dashboard solutions that meet use cases/requirements, as well as achieve ease of usability and self-service capabilities
+Analyze, trend and model modernization strategies across all macro metrics
+Work in a fast-paced Safe, Agile environment
+QUALIFICATIONS:
+Bachelor's Degree in Computer Science, Math, Data Analytics, Statistics or a related field required
+Highly skilled in Alteryx Designer required
+Highly skilled in Tableau Designer required
+Tableau and data wrangling using Alteryx experience is required
+Proficiency with SQL, R, and/or Python preferred
+7+ years of experience in finance, data &amp; analytics, and/or project management within the Financial Services industry
+Understanding of and experience with GT Modernization Strategies
+Experience with data warehouse systems, and user access, mining, and reporting applications/tools
+Flexible individual who can easily and efficiently transition across topics and disciplines
+Adept at multi-tasking and meeting deadlines in high-pressure environment
+Ability to define and track project deliveries through to implementation
+Proactive/self-starter with the ability to deliver value-added support to business partners in a dependable, timely and accurate manner
+Controls/Risk management focus - Ensure we remain adaptable and responsive to the changing regulatory landscape
+Detail oriented, adept at data organization and maintenance
+Able to work both independently and as part of a team
+Excellent time management skills and highly results oriented
+J.P. Morgan is a global leader in financial services, providing strategic advice and products to the world's most prominent corporations, governments, wealthy individuals and institutional investors. Our first-class business in a first-class way approach to serving clients drives everything we do. We strive to build trusted, long-term partnerships to help our clients achieve their business objectives.
+We recognize that our people are our strength and the diverse talents they bring to our global workforce are directly linked to our success. We are an equal opportunity employer and place a high value on diversity and inclusion at our company. We do not discriminate on the basis of any protected attribute, including race, religion, color, national origin, gender, sexual orientation, gender identity, gender expression, age, marital or veteran status, pregnancy or disability, or any other basis protected under applicable law. In accordance with applicable law, we make reasonable accommodations for applicants' and employees' religious practices and beliefs, as well as any mental health or physical disability needs.</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/rc/clk?jk=c33f36f55944233b&amp;fccid=aaf3b433897ea465&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -552,10 +730,52 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>591.4685999999999</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>6:54:45</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>Data management skills, including experience with multiple and large unstructured data sets.
 With collective experience of 50+ years in the team across business…</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>The Company
+This successful niche analytics firm, focuses on providing analytics and outsourcing solutions to clients across domains and regions.
+With collective experience of 50+ years in the team across business analytics and outsourcing, they provide on-demand analytical reports, on-demand expertise and data driven solutions to our clients.
+Their primary services include; analytical solutions to create go-to-market strategies to revive or boost product/service performance, on-demand skilled expertise, on-demand performance reporting &amp; reviews, and business process management services.
+The Role
+You will join a new Data Science team in Dubai and quickly get exposed to all facets of the business. The small team environment in Dubai will give you constant exposure to expert colleagues, business leads and customers around the world presenting a great opportunity to take your skills to the next level.
+After gaining a deep understanding of all facets of the business you will become a key member of their Data Science team who employ a full life-cycle approach from business requirement understanding, data collection and preparation to modelling and evaluation and deployment.
+You will work alongside management and Software Development team, collaborating effectively to develop and deploy new functionalities in accordance with the product road map which drive highly valuable insights to clients within the chosen sectors.
+Your work will produce tangible value for the business and its clients daily, focusing on the areas of transaction efficiency, operational process improvement and evaluation of all key business inputs.
+The Role
+2:1 or equivalent STEM degree from reputable university and A or A* in mathematics A-level, or equivalent
+3+ years? experience working with data, providing insights to business
+Excellent written and verbal communication skills across a dispersed, international organisation
+Presentation skills, including the ability to present complex topics in clear and concise reports
+Data management skills, including experience with multiple and large unstructured data sets
+Experience performing model testing, validation and writing technical documentation
+Job Owner: d.prosser</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0B4I0z8Vg4C22bXJk453pUE2nnLCUOyY_R-ihB16RDW65dAXO9w17QY8SOm2HP94HqIyiNA8KaShSf6dwMd8CjUu6RxKxZaO118H6H1vWNfYPVDJ8LaTQMcUeB7_gLkOck5nLPsEPWfOW538iyOyMgSJcZDH_Vm83mG72CpqrWi_Yp7OKsiuodxtDiAeLvZqC2PLLFl9I4EuDh-XqZnAyAMggPlQU6iOjQx04jBQuttPrNJK1kiVLjdDLLZzpgv9OH3q_b4LqnMC7aT_v727om8wApaeXwpxJHkuvYCePm-xtF8JdZC12BM9gEa_3v0GHsEYodtr593JcRyKAQDDzkXTU_XhAYoaKGjqfsU7-hbe7mokqnovfZZxNTMzokq2QjJfQNvLY7ms3aRWN4hdUXpfJzOGBE_T6kg0uoq6GxTKPMxKcOo-crKCm1AvnuO0zxO1rIKJGpUrUEY9EledQcvnaFM2BFVMDUtuWSo7Mxsg3PuGccu1smYzE7X_Hn-o8KYwJs8D7u572MJNvSHhqFzkKbyAnIQDNZ3snrJ9zjCZOnW7H4wT3KaRKl9haxbYlXo_8fY3LnGkCYRv8tcjHyHvAXSoHLYIMAI_YHLxWywmEMLIaCGasnNSl8KIhpRF2xdwZFt7AetgDgJeU8NzafjEeqlofRveztbohgqGLqDSdPewRrOKSUV&amp;p=3&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -565,23 +785,84 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Data Scientist</t>
+          <t>Data Analyst</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Barclays</t>
+          <t>NES Fircroft</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Poole BH15</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Producing meaningful data forensics to support the delivery of tuning related initiatives.
-Experimenting with and identifying various analytical methods/…</t>
+          <t>England•Remote</t>
+        </is>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Contract</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Champions data quality across systems and leads periodic data reviews and data optimization.
+Participant in data governance committees.</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Data Analyst - 12 Months Contract – Remote
+Essential: - Proficient in existing digital tools and processes (e.g. Power Automate). Experience in small to medium scale digital projects. A working knowledge of software programming. Experience in data mining and analysing. Understanding of machine-learning and operations research. Experience using business intelligence tools and data frameworks. Data Modelling to create Algorithms and predictive models.
+JOB SUMMARY
+The Data Analyst is responsible for addressing critical data-related business problems by creating strategies, to analyse, connect and draw conclusions from clients systems, data lakes and external sources using robust data science techniques. Working with Business subject matter experts, the role will be familiar with labelling standards and compliance measures and will play a key role in supporting portfolio decision making and process development.
+The Data Analyst is also a critical contributor to discussions around data architecture and standards led by Information Management (IM) and Digital.
+The Data Analyst interprets and analyses data to provide innovative solutions to problems, designs data modelling processes to create algorithms and predictive models or performs custom analysis as required. The Data Analyst will support and/or lead initiatives relating to machine learning and artificial intelligence, representing GRA in discussions with Information Management and Digital.
+The Data Analyst will be responsible for effective compliance monitoring and support time-critical provision of analysis of labelling data.
+The role also acts as a key interface with IM providing SME for system requirements and data quality. In addition, you will be expected to lead or participate in imitative to improve efficiencies.
+JOB RESPONSIBILITIES
+Proactively identify and extract valuable data from multiple sources and automate collection processes
+Participant in data governance committees
+Undertake pre-processing of structured and unstructured data
+Sift and analyse data from multiple angles, looking for trends that highlight problems or opportunities
+Builds and implements predictive models and machine-learning algorithms
+Use a combined knowledge of computer science and applications, modelling, statistics, analytics and maths to solve problems
+Maintain effective relationships with other platform lines and Business Units enabling facilitation of effective portfolio delivery
+Present information using data visualization techniques
+Become a subject matter expert in 1-2 digital. Automation skillsets (e.g. functionality mapping, predictive analysis)
+Create awareness by working across functions to share and learn about best practices.
+Lead or participate in ILG and or GRO technology initiatives
+Developing best suited data models and algorithms in collaboration with Information Management and Digital partners
+Assessing the effectiveness of the data model with the ability to select the right technique of data gathering.
+Champions data quality across systems and leads periodic data reviews and data optimization
+Point of contact for labelling compliance data.
+Takes appropriate risks to advance new concepts and methodologies for the design and optimization of data analytic projects.
+Use modelling to create the optimized customer experience.
+QUALIFICATIONS / SKILLS
+Proven experience as a Data Analyst or Data Scientist
+Proficient in existing digital tools and processes (e.g. Power Automate)
+Connective thinker, able to challenge and suggest optimization through data and insights.
+Experience in small to medium scale digital projects.
+A working knowledge of software programming
+Experience in data mining and analysing
+Understanding of machine-learning and operations research
+Experience using business intelligence tools and data frameworks
+Analytical mind and business acumen
+Strong math skills (e.g. statistics, algebra)
+Problem-solving aptitude
+Ability to be flexible, adapt to change work independently, as well as part of a team in a matrix environment.
+BSc/BA in Computer Science, or relevant field; graduate degree in Data Science or another quantitative field is preferred
+Candidates must be eligible to work in the UK
+With over 90 years' combined experience, NES Fircroft (NES) is proud to be the world's leading engineering staffing provider spanning the Oil &amp; Gas, Power &amp; Renewables, Infrastructure, Life Sciences, Mining, Automotive and Chemicals sectors worldwide.With more than 100 offices in 45 countries, we are able to provide our clients with the engineering and technical expertise they need, wherever and whenever it is needed. We offer contractors far more than a traditional recruitment service, supporting with everything from securing visas and work permits, to providing market-leading benefits packages and accommodation, ensuring they are safely and compliantly able to support our clients.</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DiSGR40Z5TcCdl_J7A59VP_6ZDYIBt_zfNy0x5FbgpmDCyNykNdPc5kBSuTvSlweuLX7JnAe9oDhaM7icfTJ3MlVH4ryhWuJnpY1u7yEZY9DNdWvmFV2ydQfRpBFJWVpQCJYRLYFfeoufehI86UDd5kGewKnZ74pi1pthtszICjrdKwvJTb1zqtEgoIkq708TEt0e3VpVFGHuzCxmbEkDXZuFiQpwlmVe6_zlgT3QIoZLsTaQFmDxdFpC7zXsKBaKzrVsXNgEzjxty_3FdmIYVWeEVvYABZSDaB4fbRoVp3V7EunMPRAcXs5niGuXWFHRanU-DmpJilDbgsogLVCHmBQ1_4k4PppwNw9ot0f8WuqcLdP6INXFt64LWdvBz2lhLe4HB-qDmbVzt2iPaUMe0ZPdFz5B1nKINwOINNw-6Ok0-79qAmmBJNfeCPqQFlBKk1y1PugyJcSxuM7_4123LfxXQWCpANfGMpZgtb7gudXZJz8lSc_--91rMRhDJrWZ_0HJ0LHTjsOajnR0AmqeTr0xTzOSR0sTZu3ug-08XcQkri6oUuVJTU1Iz2m7FQvH_aCLe_7vUQ71Eukh8GeSePJU1YCTiZU4CYQ821lljFWD2V5q3xtLcFCnuqnSUTnQ=&amp;p=4&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -591,22 +872,74 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Senior Data Scientist</t>
+          <t>Product Manager - Unity Platform: Intelligence &amp; Analytics</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Metrica Recruitment</t>
+          <t>JPMorgan Chase Bank, N.A.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>You will be involved in the data-mining, machine learning and graph analysis techniques for a variety of modelling problems involving customers, their…</t>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Full-time, Permanent</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>9.039200000000001</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0:14:30</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Conducting research and providing ideas on using Unity data to develop analytics to identify process improvements and new client opportunities.</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Department and program description
+The Interaction Management Program consists of a portfolio of initiatives aimed at transforming and delivering better ways of working for DPS Operations when they interact with each other and with their clients. The Interaction Management team is a dedicated group of Product and Program managers focused on managing a broad product portfolio, including daily operational support of existing products, and initiatives that support the transformation of the operational landscape. As a team we are focused on outcomes, being data driven, learning through experimentation, and collaboration with cross functional teams including Technology, User Experience Researchers &amp; Designers, Data Science, Product Marketing and Operations.
+The Interactions Management team aims to improve the Operations user experience through the design, development and delivery of a suite of capabilities that leverage new technologies to address operational needs when managing the resolution of exceptions and enquiries. Delivery of these capabilities will empower users to make process changes, enhance controls, create resource capacity, enable better analytics, and improve the user and client experience.
+Unity will be the CIB cross-LOB enquiry and exception case management platform removing the need for LOBs to build separate case management systems. Unity will be an open platform, allowing LOBs to connect to it in the manner that suits them best.
+Role description
+The successful applicant will be part of a global product team responsible for the delivery of Unity - the new cross-CIB case management platform to be used initially by CIB Operations. The individual will support with the delivery of Unity intelligence and analytics capabilities, partnering closely with the Unity Product Managers, Technology, User Experience Researchers &amp; Designers, Data Science and Operations teams. Responsibilities include:
+Participating in the delivery of the Unity Intelligence &amp; Analytics product roadmap; from ideation to setting priorities for planning and execution
+Identifying business needs, detailing business requirements, and partnering with Design,Technology and Data Science teams to deliver the product capabilities
+Applying agile methodologies (i.e. writing EPICs user stories etc.) highlighting the value delivered by each requirement and release
+Conducting research and providing ideas on using Unity data to develop analytics to identify process improvements and new client opportunities
+Contributing to the user outreach strategy &amp; rollout in partnership with client service teams
+Building and maintaining relationships with stakeholder groups, and promoting the Unity brand and product
+Work across global Risk, Legal and Compliance organizations to ensure functionality is fully compliant with all regulatory and data privacy requirements
+Required skills and qualifications
+Prior experience of Product Management in financial services
+Experience managing strategic product development and process re-engineering initiatives
+Prior experience and understanding of CIB Operations business areas and trade lifecycle knowledge preferred
+Ability to build solid relationships within a short time period
+Excellent communication skills
+Structured approach to problem solving, and decision-making
+Attention to detail, seek out potential problem area, conduct root cause assessment and synthesize findings to formulate recommendations
+Prioritisation and organisational skills
+Ability to work under pressure to meet deadlines
+Curious, inquisitive and motivated to deliver value to users &amp; clients
+This role provides an excellent platform to be involved in the transformation agenda across the CIB, D&amp;PS and LOBs.
+J.P. Morgan is a global leader in financial services, providing strategic advice and products to the world's most prominent corporations, governments, wealthy individuals and institutional investors. Our first-class business in a first-class way approach to serving clients drives everything we do. We strive to build trusted, long-term partnerships to help our clients achieve their business objectives.
+We recognize that our people are our strength and the diverse talents they bring to our global workforce are directly linked to our success. We are an equal opportunity employer and place a high value on diversity and inclusion at our company. We do not discriminate on the basis of any protected attribute, including race, religion, color, national origin, gender, sexual orientation, gender identity, gender expression, age, marital or veteran status, pregnancy or disability, or any other basis protected under applicable law. In accordance with applicable law, we make reasonable accommodations for applicants' and employees' religious practices and beliefs, as well as any mental health or physical disability needs.</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/rc/clk?jk=36447c0457e010f9&amp;fccid=aaf3b433897ea465&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -616,122 +949,75 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Head of Data Science</t>
+          <t>CIB - Interaction Management - Unity Reporting &amp; Analytics P...</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Metrica Recruitment</t>
+          <t>JPMorgan Chase Bank, N.A.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>You will do this through your deep understanding of data and what it can do, your ability to understand the business context of that data, the process of…</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Modernization Data Scientist/Visualization - VP</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>JPMorgan Chase Bank, N.A.</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
           <t>Bournemouth</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Modify and blend data by designing workflows in the Alteryx application to harvest, validate, clean and standardize data in a highly repeatable manner.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Product Manager - Unity Platform: Intelligence &amp; Analytics</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>JPMorgan Chase Bank, N.A.</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Bournemouth</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Conducting research and providing ideas on using Unity data to develop analytics to identify process improvements and new client opportunities.</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>CIB - Interaction Management - Unity Reporting &amp; Analytics P...</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>JPMorgan Chase Bank, N.A.</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Bournemouth</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Full-time, Permanent</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>9.039200000000001</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0:14:30</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>As a team we are focused on outcomes, being data driven, learning through experimentation, and collaboration with cross functional teams including Technology,…</t>
         </is>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>CfACTs Research Fellow (Framestore 1 Project) - Application...</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Bournemouth University</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Dorset</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>This often includes difficult to solve light transport situations such as nested dielectric media, volumetric multiple scattering and complex lighting scenarios…</t>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Department and program description
+The Interaction Management Program consists of a portfolio of initiatives aimed at transforming and delivering better ways of working for DPS Operations when they interact with each other and with their clients. The Interaction Management team is a dedicated group of Product and Program managers focused on managing a broad product portfolio, including daily operational support of existing products, and initiatives that support the transformation of the operational landscape. As a team we are focused on outcomes, being data driven, learning through experimentation, and collaboration with cross functional teams including Technology, User Experience Researchers &amp; Designers, Data Science, Product Marketing and Operations.
+The Interactions Management team aims to improve the Operations user experience through the design, development and delivery of a suite of capabilities that leverage new technologies to address operational needs when managing the resolution of exceptions and enquiries. Delivery of these capabilities will empower users to make process changes, enhance controls, create resource capacity, enable better analytics, and improve the user and client experience.
+Unity will be the CIB cross-LOB enquiry and exception case management platform removing the need for LOBs to build separate case management systems. Unity will be an open platform, allowing LOBs to connect to it in the manner that suits them best.
+Role description
+The successful applicant will be part of a global team responsible for the delivery of Unity - the new cross-CIB case management platform to be used initially by CIB Operations. The individual will manage the delivery of Unity reporting and analytics capabilities, partnering closely with the Unity Product Managers, Technology, User Experience Researchers &amp; Designers, and Operations teams. Responsibilities include:
+Defining key aspects of the product strategy and implementation phases; from ideation to setting priorities for planning and execution
+Driving the product roadmap, detailing business requirements and partnering with Design and Technology teams to deliver the product capabilities
+Applying agile methodologies (i.e. EPICs, user stories etc.) highlighting the value delivered by each requirement and release
+Conducting research and study on best in class reporting and analytics capabilities
+Contributing to the user outreach strategy &amp; rollout in partnership with client service teams
+Owning the OKRs for the Unity reporting and analytics
+Building and maintaining relationships with stakeholder groups, and promoting the Unity brand and product
+Responsible for a team of Unity reporting and analytics product owners
+Required skills and qualifications
+Prior experience of Product Management in financial services
+Experience managing strategic product development and process re-engineering initiatives
+Prior experience and understanding of CIB Operations business areas and trade lifecycle knowledge preferred
+Ability to build solid relationships within a short time period
+Excellent communication skills
+Structured approach to planning, problem solving, and decision-making
+Attention to detail, seek out potential problem area, conduct root cause assessment and synthesize findings to formulate recommendations
+Prioritisation and organisational skills
+Ability to work under pressure to meet deadlines
+Curious, inquisitive and motivated to deliver value to users &amp; clients
+This role provides an excellent platform to be involved in the transformation agenda across the CIB, D&amp;PS and LOBs.
+J.P. Morgan is a global leader in financial services, providing strategic advice and products to the world's most prominent corporations, governments, wealthy individuals and institutional investors. Our first-class business in a first-class way approach to serving clients drives everything we do. We strive to build trusted, long-term partnerships to help our clients achieve their business objectives.
+We recognize that our people are our strength and the diverse talents they bring to our global workforce are directly linked to our success. We are an equal opportunity employer and place a high value on diversity and inclusion at our company. We do not discriminate on the basis of any protected attribute, including race, religion, color, national origin, gender, sexual orientation, gender identity, gender expression, age, marital or veteran status, pregnancy or disability, or any other basis protected under applicable law. In accordance with applicable law, we make reasonable accommodations for applicants' and employees' religious practices and beliefs, as well as any mental health or physical disability needs.</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/rc/clk?jk=710caae206b49a82&amp;fccid=aaf3b433897ea465&amp;vjs=3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
improved travel time, started adding multi-page search
</commit_message>
<xml_diff>
--- a/Indeed_WebScrape/jobsDf.xlsx
+++ b/Indeed_WebScrape/jobsDf.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,76 +491,50 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sr. Data Scientist (Remote)</t>
+          <t>Data Entry For Accountancy</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CrowdStrike</t>
+          <t>SC Business Services Limited</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>United Kingdom•Remote</t>
+          <t>Poole BH15</t>
         </is>
       </c>
       <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Part-time, Permanent</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Have experience working on very large data sets of sparse high dimensional data and experience in pre-processing and analyzing such data to gain actionable…</t>
+          <t>Must have good accurate typing skills, and willing to learn.
+The hours will be set part time Hours Between Monday and Friday.
+Part-time hours: 20 per week.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>At CrowdStrike we’re on a mission - to stop breaches. Our groundbreaking technology, services delivery, and intelligence gathering together with our innovations in machine learning and behavioral-based detection, allow our customers to not only defend themselves, but do so in a future-proof manner. We’ve earned numerous honors and top rankings for our technology, organization and people – clearly confirming our industry leadership and our special culture driving it. We also offer flexible work arrangements to help our people manage their personal and professional lives in a way that works for them. So if you’re ready to work on unrivaled technology where your desire to be part of a collaborative team is met with a laser-focused mission to stop breaches and protect people globally, let’s talk.
-About the Role:
-CrowdStrike EndPoint Protection team is expanding. We are looking for data scientists to help us build solutions with detections based on indicators of risk, analytics and risk scoring. You will have the opportunity to apply your coding, mathematical and scientific research skills to the bleeding edge of security technology. You’ll be able to leverage large-scale rich data to meaningfully improve our supervised learning models and refine our identification of malicious computer software and behavioral threats. CrowdStrike’s cybersecurity data is one-of-a-kind: we process over 1 trillion behavioral events per day and have over 2000 terabytes of malware samples in our research repository. We are a diverse and multidisciplinary team, and you’ll have the chance to broaden your horizons by working jointly with a team of Big Data, Machine Learning, and Security domain experts on hard and impactful problems.
-What You'll Need:
-Undergraduate or postgraduate degree in a STEM field
-Extensive post/undergraduate experience in data science, machine learning, or any field employing computational science or data driven analyses
-Programming experience in Python or Scala
-You will:
-Mine large scale and high dimensional data, identify patterns, and visualize trends
-Create predictive models using supervised learning techniques to detect and stop the most sophisticated threats
-Innovate new semi-supervised and online learning techniques to enhance our threat detection capabilities and reduce nuisance false positives for our customers.
-Work closely with domain experts to improve our raw data and to derive more value from data collected
-Hone your ability to balance detail-oriented research with goal-oriented business objectives
-Implement and experiment with new algorithms and methodologies to help improve our machine learning models
-Automate and visualize analyses, results and processes in our machine learning pipeline
-You are:
-Passionate about cybersecurity, with a firm understanding of the problem space or passionate about applying your machine learning skillset to new domain areas such as cybersecurity
-Versed in utilizing Machine Learning techniques and familiar with the standard algorithms, their trade-offs, their usage, and how to tune them
-Have experience working on very large data sets of sparse high dimensional data and experience in pre-processing and analyzing such data to gain actionable insights
-An independent self-starter who likes to take ownership and independently seeks out new challenges
-Thirsty for knowledge and do not hesitate to step outside of your comfort zone to learn new technologies, algorithms and concepts
-Comfortable to dive into a Python codebase, including experience with unit testing and the python packaging ecosystem
-Comfortable and experienced working in a Linux environment in the AWS cloud
-Analytically minded: never afraid to drill down into a data-set, or debug-deeper into an unfamiliar codebase
-#LI-MC1
-#LI-Remote
-Benefits of Working at CrowdStrike:
-Market leader in compensation and equity awards
-Competitive vacation policy
-Comprehensive health benefits
-Flexible work environment
-Wellness programs
-Stocked fridges, coffee, soda, and lots of treats
-We are committed to building an inclusive culture of belonging that not only embraces the diversity of our people but also reflects the diversity of the communities in which we work and the customers we serve. We know that the happiest and highest performing teams include people with diverse perspectives and ways of solving problems so we strive to attract and retain talent from all backgrounds and create workplaces where everyone feels empowered to bring their full, authentic selves to work.
-CrowdStrike is an Equal Opportunity employer. All qualified applicants will receive consideration for employment without regard to race, color, religion, sex including sexual orientation and gender identity, national origin, disability, protected veteran status, or any other characteristic protected by applicable federal, state, or local law.</t>
+          <t>We are looking for a data entry person to work within our small growing Accountancy firm.Must have good accurate typing skills, and willing to learn.The hours will be set part time Hours Between Monday and Friday.We are based in Poole Town Centre.Pay will be confirmed at interview stage.Part-time hours: 20 per weekJob Types: Part-time, PermanentSchedule:Day shiftMonday to FridayNo weekendsWork remotely:No</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0BJMW_X9OCLkZ04_weh8WkR-IGNb1MhigwTP7XGwrJOF_X_VSZLnRc8x9p7EGl99QfnO7rcpARi_jZFAi1DQHRR86_6bF7GzryOxmNFcCt0jbPYDtl2FnYUy7DwD_4SPcZwsD3f4vyYqLRca812fYP7F8n8_9C7erjuqEi08KoOkZEWVoCL6ai9QF3kCu8rhr_ShSOywtbPRt4zaE8GaodWl1-xjz9b5wIOozBirZ7HqTDfPDi7pYZFyYc0FId_otSUUkyVYr1cyfufrqZ7yMHchJ3YXZoWbYYgAx6_NHuBaUQ8uA4Bbj_57GjLTgwojtROjLSSfrrN4ciZ24qAbkb4RU23x6_vs9227DGA_ZiHD3gURO6zjohAXaDDquJHmNn8OraSx4m9Kt0Wgb_YN5reMY9wgDVHBJJIvzyzhyQM0CKWGg3UCLAGPiIupJRWa9CL0LOgxIWs0zdD5UtTQaLuwGkmrL4Y2YAAgq8O-yocvVAEie4PCy6ccYf-_btGfToUYsSIMT_DcVtRcM3lnE9l0OgTk9wMgEnxlvdHv9jVeOhmUpP4wrXo&amp;p=0&amp;fvj=0&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DLumFLdxabPOXZwbbSci2buojfI0jQd0LQBmxSLF1k3Ft1tKzY1KGYcLNIyU2uhqv6inY4pnqn9kK8rhcSvDZSygvMCeIIYvFCp5czzevS9ks7xXfL-bReWujjRJYf7Yd0DjfAQnOOVZ5AIJCP527XwcaJzk-OW42d2p7fYxEW6g9dIFszajSdqHTFhUDE4X3baa8aiF7Sbqp-vY2J5waH0Qo5y_XLN1ajo-1JXDrAs9hVNY7LegYXKaDvF_3JMzJPoRh6yr8zVaDMzZlDxFZ-fLZuEsIS451rfmSbXyxS5mCx1bNsLOj3em80yhmitF8MGcrKHizmlkxf9EhNAeahkgTE84XGmvyqs2gsBEnEny0zjMqrQLEh91nGdklHGDylVWReAWJ-oHt7YUDQPQbRrjBbLiVw1a4e_lYPHwjEhqpInvZhgbAhbqTLrPgx9eo_CDv4oeH2cbzoFvqh2QS1wpc4jCYtLcs=&amp;p=0&amp;fvj=1&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -570,60 +544,49 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Defence Data Scientist</t>
+          <t>Data Engineer</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Metrica Recruitment</t>
+          <t>Kortext</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>South West</t>
+          <t>Bournemouth</t>
         </is>
       </c>
       <c r="E3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>£40,000 - £45,000 a year</t>
+          <t>£25,000 - £35,000 a year -  Full-time, Permanent</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>167.4113</v>
+        <v>9.039200000000001</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2:20:06</t>
+          <t>0:14:30</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Three years' or more of experience in data science.
-Your role would be to develop and design decision aid tools and models to carry out analysis for customers…</t>
+          <t>Frastructure required for optimal extraction, transformation, and loading of data from a wide variety of data sources.
+An advanced understanding of SQL.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>The Company
-This highly successful strategy consultancy specialise in the government and defence sectors.
-They have significant innovation funding from the MoD, meaning that they don't just pitch an idea to improve what's in place but actually have to prove that something has never been done before and is genuinely different to anything or anyone else.
-The Role
-Your role would be to develop and design decision aid tools and models to carry out analysis for customers and more recently, there has been an increased focus on product development. The content of decision aids, used for strategic or operational decision making, is predominantly AI based machine learning and there are a range of unique techniques developed internally.
-A niche but exciting area they work in is explainable AI, which is a part of past, current projects and future plans. Given that clients are typically within the defence sector, when machine learning algorithms spit out an answer, it's not possible to simply rely on the computer saying this is what you should do. It's essential to add reasons why, which is challenging to generate from standard ML algorithms.
-The Individual
-Three years' or more of experience in data science.
-Strong Python proficiency.
-Excellent communication skills, both verbal and written.
-To acquire security clearance, it's a necessity that you have lived in the UK for five consecutive years without spending more than three consecutive months out of the UK.
-Job Owner: d.prosser</t>
+          <t>Job Description – Data Engineer Summary Kortext is the UK’s leading eTextbook provider, serving universities globally. We are recruiting a Graduate Data Engineer to help us scale our business and products as we grow both in the UK and internationally.Kortext has seen significant growth in the last 12 months and this role is key to driving our expansion by continuing to build on this success. The ideal candidate is a graduate with a background in Computer Science and/or Data Analysis who is enthusiastic and keen to learn. They will support and implement data initiatives both internal and customer facing and report into our Senior Data Engineers.Key Responsibilities · Create and maintain optimal data pipeline architecture· Identify, design, and implement internal process improvements: automating manual processes, optimizing data delivery, re-designing infrastructure for greater scalability, etc.· Build analytics tools that utilize the data pipeline to provide actionable insights into customer acquisition, operational efficiency, and other key business performance metrics.· Delivering Business Intelligence and Data Engineering Projects.· frastructure required for optimal extraction, transformation, and loading of data from a wide variety of data sources.· Build the infrastructure required to implement a Data Estate.Education &amp; Experience · Bsc/BA in Computer Science/Software Engineering or other Data related degree.Technical skills · An appreciation of data warehouse design (e.g. dimensional modeling)· Familiarity with BI technologies (e.g. Microsoft Power BI, Azure Analysis Services, Tabular Models/DAX).· An advanced understanding of SQL.· Experience with Python/R and other languages, knowledge of C# and Web APIs would be beneficial.Personal Characteristics · Proven abilities to take initiative and be innovative.· Analytical mind with a problem-solving aptitude.· Committed to excellence, self-starter who is hungry to learn.· Meticulous and excellent attention to detail.· The ability to work collaboratively as part of a close-knit team and manage themselves in a non-office-based work environment.Job Types: Full-time, PermanentSalary: £25,000.00-£35,000.00 per yearAdditional pay:Bonus schemeBenefits:Private medical insuranceWork from homeSchedule:Monday to FridayWork remotely:No</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0B4I0z8Vg4C22bXJk453pUE2nnLCUOyY_R-ihB16RDW65dAXO9w17QY8SOm2HP94HptMLXv5tQJz9tiF4ev5eCB4EYCTHe-YzBJKwMAnjDabRN056LgA49BqFgm_-BvDdVh6acr-5rEEdCObYarf9kGPomUSuya6N7oGNCnjHCdq9tr4EL2gSBmLJVWksWww70M6mRt-8ofZNSeK88XLYo70iucoBUsTk7ten_BnhCwp-5VRI35IL30_VeyFxJCYZKdoP_eXYl_kV6h8td3TOJKlxHT02CYMUp1BZVu5T4SvsV4i1aoJ1yoRAOwdfA-pnVpiEum2s4kG0Q_Pvnmr8DdG1DWtlKxDsTi_JwGfNBxq2DG3UeGtKv--EILNyxnRqeGqsARsahpMpvkBKh4AlmRco_16hSvNz298hE8C_0iigU7LBYbzZvpxydY0ZUtSmg1F_N3DqqLabb6HT-1yjCoxKcO5Kup1YXP3YyoTTxrM3gBQlWrRM1O6Z-N7MGIyhgs6AvCIXU0YMfe6rMG3S349bxA6W-9JjTP2IJrPbNE4lyPZD8vmEhR5i6Kj52WF7iubM5AzYUPShWPaiGf9qzoHAxi83K4QvjNk2jHJ8h1OQPQe1EDqLmPKr_Wo3cTvyooN77J1PGn2vZdYXNIKyDu7lrtxBPO0V8tIOUZeFMjqmd8AIBIw0iePRz_MfOrmFk=&amp;p=1&amp;fvj=0&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0ATA-436Np_sDHyRyXgfnC7rulQh_HAeSRkBVkE7CpmFpvNpKLrqjOCQMUHWE6D8TXEKgbjyQI1Y_dDWC7IdAq4vkRD5-ugcoLNxgWdYUaeFM9JWbxHMwO8CoqzBurJQma5b6I9Jvkyg5wJVz-FztZQd4OmsxU0oT9F5u_DvyqSTdK4yxojmMUZlCdJUxYFy6zXfF_c1As1Ug65bEscz8onSVvWcuGmS921-4DwDOrv3VwyAdh271PJ90sNVyYvAQGQpTWE1MhsPPlZ-9OgQqLEFipe0bRYOV8XML5aB0CbsgNdV8nOvPgHgwYSXu6fOfSj0pNFPUDK-4anYqGhCzH9seV7XDS36hw3dRzaZQJeadOHJ8tlT-g3-FRYNP5ZgHjR6345yHZjtEJ7TtDNg8KDXP7_1wQ3tgcx23tiDzQ8TmnUBVqraJQc3XtHQU-Dah_evbW8xqEkzXIYyUJCDPULDiYqzv_JfjA=&amp;p=1&amp;fvj=1&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -633,81 +596,43 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Modernization Data Scientist/Visualization - VP</t>
+          <t>Database Developer</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>JPMorgan Chase Bank, N.A.</t>
+          <t>Bournemouth Independent Group</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Bournemouth</t>
+          <t>Bournemouth+1 location</t>
         </is>
       </c>
       <c r="E4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Full-time, Permanent</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>9.039200000000001</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0:14:30</t>
-        </is>
-      </c>
+          <t>£40,000 - £50,000 a year</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Modify and blend data by designing workflows in the Alteryx application to harvest, validate, clean and standardize data in a highly repeatable manner.</t>
+          <t>Data migration and data integrity.
+The ideal candidate for this role is someone with a solid understanding of database principals, a love of data, reporting and…</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>This position will be a Tableau &amp; Alteryx Dashboard Developer for the Corporate Technology Office (CTO) dashboards, which will directly report to the CTO Portfolio Insights Product Owner and will partner closely with the CTO Modernization Execution leads. The remit will encompass all end to end requirements to prioritization, planning and execution of work inclusive of infrastructure design, test execution, and implementation. The successful candidate must possess strong analytical &amp; problem-solving skills, have the ability to prioritize and manage time.
-KEY RESPONSIBILITIES:
-Develop dynamic, scalable and effective dashboards in Tableau using Alteryx and other data wrangling tools to summarize and analyze key business drivers using Safe, LEAN, Agile methodologies
-Leverage a strong foundational knowledge of financial, application and developer metrics to build effective solutions that simplify, automate, and add value
-Create robust and stable data pipelines as well as efficient data maps for optimal Tableau performance
-Express creativity and ingenuity to transform how we see and understand data
-Perform data integration, write efficient SQL Queries, and develop/deploy reporting solutions that apply data visualization standards and best practices, and meets quality standards by performing unit testing
-Query with SQL or Python scrips, configure APIs used to connect data sources.
-Modify and blend data by designing workflows in the Alteryx application to harvest, validate, clean and standardize data in a highly repeatable manner
-Understand the variety of sources for information and how to strategically source data
-Tracking development and deployment timelines
-User Acceptance Testing and Validation of new dashboards
-Gather, interpret and analyze business requirements and use cases and design dashboard solutions that meet use cases/requirements, as well as achieve ease of usability and self-service capabilities
-Analyze, trend and model modernization strategies across all macro metrics
-Work in a fast-paced Safe, Agile environment
-QUALIFICATIONS:
-Bachelor's Degree in Computer Science, Math, Data Analytics, Statistics or a related field required
-Highly skilled in Alteryx Designer required
-Highly skilled in Tableau Designer required
-Tableau and data wrangling using Alteryx experience is required
-Proficiency with SQL, R, and/or Python preferred
-7+ years of experience in finance, data &amp; analytics, and/or project management within the Financial Services industry
-Understanding of and experience with GT Modernization Strategies
-Experience with data warehouse systems, and user access, mining, and reporting applications/tools
-Flexible individual who can easily and efficiently transition across topics and disciplines
-Adept at multi-tasking and meeting deadlines in high-pressure environment
-Ability to define and track project deliveries through to implementation
-Proactive/self-starter with the ability to deliver value-added support to business partners in a dependable, timely and accurate manner
-Controls/Risk management focus - Ensure we remain adaptable and responsive to the changing regulatory landscape
-Detail oriented, adept at data organization and maintenance
-Able to work both independently and as part of a team
-Excellent time management skills and highly results oriented
-J.P. Morgan is a global leader in financial services, providing strategic advice and products to the world's most prominent corporations, governments, wealthy individuals and institutional investors. Our first-class business in a first-class way approach to serving clients drives everything we do. We strive to build trusted, long-term partnerships to help our clients achieve their business objectives.
-We recognize that our people are our strength and the diverse talents they bring to our global workforce are directly linked to our success. We are an equal opportunity employer and place a high value on diversity and inclusion at our company. We do not discriminate on the basis of any protected attribute, including race, religion, color, national origin, gender, sexual orientation, gender identity, gender expression, age, marital or veteran status, pregnancy or disability, or any other basis protected under applicable law. In accordance with applicable law, we make reasonable accommodations for applicants' and employees' religious practices and beliefs, as well as any mental health or physical disability needs.</t>
+          <t>Database Developer · Rare opportunity to make a real difference!· Great Benefits· Training &amp; Professional Development Opportunities· Up to £50,000 DOE including a Performance Bonus!THE GROUPWe are BIG - a friendly and fun award-winning Bournemouth based team providing some of the most comprehensive and competitive household insurance and maintenance products. We’re one of the fastest-growing providers of these services within the sector – a group with a mission to expand further on a national and international scale!We are a team, first and foremost. Our team strives to be at the forefront of technological improvement in our market sectors. We built the number one ranked gadget insurance site, we've developed amazing cutting edge product technology and we're currently working on (amongst many other things) creating the world largest consumer brand within its market in cooperation with some amazing agencies.THE ROLEWe are looking for a talented Database Developer to augment our fast growing, experienced and energetic team. You should be logical and mathematical in thought and passionate in your approachYou will work with your team to deliver new amazing or improved systems. The ideal candidate for this role is someone with a solid understanding of database principals, a love of data, reporting and experienced in this field of work. Commercial awareness of the financial services and home services industries would be a desirable plus! The role covers the full database life-cycle process and will involve customer facing interaction, working with the business from requirements through to delivery, reporting and future enhancements.SKILLS NEEDED· Microsoft SQL Server· SSMS.· Backups, Restores and Disaster recovery processes.· Analytics and reporting using systems such as SSRS.· Data migration and data integrity.· Cloud based databases and storage.BENEFITSWe work to ensure everyone reaches their potential and thrives on what they’ve accomplished. We offer whatever we can to motivate your development by applying rigorous well founded techniques, such as ensuring you enjoy time with your colleagues by paying for your fun nights out, health and fitness access and much more.Remuneration!Up to £50,000 per annum (DOE) inclusive of a 10% Performance bonus + Benefits + Being part of an awesome company which make real progressive changes on a daily basis!Job Type: Full-timeSalary: £40,000.00-£50,000.00 per yearEducation:Bachelor's (preferred)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/rc/clk?jk=c33f36f55944233b&amp;fccid=aaf3b433897ea465&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CRHxVuVxA7tmydCDz81QEwDiUTiGapFnr4O75YEF9YodcwR6nhSyZvzmjkUi-Xc1CqIJQfHOT8BNBtzgDyVeEVCQO2l-bkjBJmjyKESwz9YvO1CCjwllHRZOE9i6MvEllMX-siifT9sH33eb37idOwphUSfgozAFD1xUk4PR_7Y46SJBJUAf2IuJYkDlfHcDT0DokzRx8Wri0qgYBV-NBnBE7RK9ll54gXF0_UTDhMA6-6rRHDwHkRLRW4a3ykhD4Alca0EJ6qf2BqoTXacNiRgkWCjzUaLQlMwySkIfxkLAIVPyj52o8PraIOC4dJzOBZVzodl-JQEb1a8XDOWwPexGSx8Tadokyk_5ZBHs0i5mkaW3gJGtCf8raeSbAKYI9q4wVyTM7NsF7dSw3OwlH7-YBu3_PZ6vkJnQ3MYR-QzUThupYUEv-fTc6vCEPx0zfSJXzDn-Nbq1rKlEzw5EP-RnlYD09cwZg=&amp;p=2&amp;fvj=1&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -717,65 +642,42 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Data Scientist</t>
+          <t>Graduate Data Engineer</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Metrica Recruitment</t>
+          <t>Kortext</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Christchurch+1 location</t>
         </is>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>591.4685999999999</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>6:54:45</t>
-        </is>
-      </c>
+          <t>£24,000 - £27,000 a year -  Full-time, Permanent</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Data management skills, including experience with multiple and large unstructured data sets.
-With collective experience of 50+ years in the team across business…</t>
+          <t>The ideal candidate is an experienced data pipeline builder and data wrangler who enjoys optimizing data systems and building them.</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>The Company
-This successful niche analytics firm, focuses on providing analytics and outsourcing solutions to clients across domains and regions.
-With collective experience of 50+ years in the team across business analytics and outsourcing, they provide on-demand analytical reports, on-demand expertise and data driven solutions to our clients.
-Their primary services include; analytical solutions to create go-to-market strategies to revive or boost product/service performance, on-demand skilled expertise, on-demand performance reporting &amp; reviews, and business process management services.
-The Role
-You will join a new Data Science team in Dubai and quickly get exposed to all facets of the business. The small team environment in Dubai will give you constant exposure to expert colleagues, business leads and customers around the world presenting a great opportunity to take your skills to the next level.
-After gaining a deep understanding of all facets of the business you will become a key member of their Data Science team who employ a full life-cycle approach from business requirement understanding, data collection and preparation to modelling and evaluation and deployment.
-You will work alongside management and Software Development team, collaborating effectively to develop and deploy new functionalities in accordance with the product road map which drive highly valuable insights to clients within the chosen sectors.
-Your work will produce tangible value for the business and its clients daily, focusing on the areas of transaction efficiency, operational process improvement and evaluation of all key business inputs.
-The Role
-2:1 or equivalent STEM degree from reputable university and A or A* in mathematics A-level, or equivalent
-3+ years? experience working with data, providing insights to business
-Excellent written and verbal communication skills across a dispersed, international organisation
-Presentation skills, including the ability to present complex topics in clear and concise reports
-Data management skills, including experience with multiple and large unstructured data sets
-Experience performing model testing, validation and writing technical documentation
-Job Owner: d.prosser</t>
+          <t>Job Description – Graduate Data EngineerSummaryKortext is the UK’s leading eTextbook provider, serving universities globally. We are recruiting a Data Engineer to maintain and optimize our data and data pipeline architecture.Kortext has seen significant growth in the last 12 months and this role is key to driving our expansion by continuing to build on this success. The ideal candidate is an experienced data pipeline builder and data wrangler who enjoys optimizing data systems and building them. The Data Engineer will also support and implement data initiatives, internal and customer facing business intelligence products. They must be self-directed and comfortable supporting the data needs of multiple teams, systems and products.Key Responsibilities· Create and maintain optimal data pipeline architecture· Identify, design, and implement internal process improvements: automating manual processes, optimizing data delivery, re-designing infrastructure for greater scalability, etc.· Build the infrastructure required for optimal extraction, transformation, and loading of data from a wide variety of data sources.· Build the infrastructure required to implement a Data Estate.· Build analytics tools that utilize the data pipeline to provide actionable insights into customer acquisition, operational efficiency and other key business performance metrics.· Work with stakeholders including the Executive, Product, Data and Design teams to assist with data-related technical issues and support their data infrastructure needs.· Keep our data secure and ensure its storage is compliant with data protection rules and regulations.· Create data tools for analytics members that assist them in building and optimizing our product into an innovative industry leader.· In depth knowledge of data protection, and security protocols related to data integrity.Education &amp; Experience· Bsc/BA in Computer Science, Engineering or significant industry experience· An interest in building and optimizing data pipelines, architectures, and data sets.· An interest in performing root cause analysis on internal and external data and processes to answer specific business questions and identify opportunities for improvement.· A knowledge or basic understanding of SQL· Willingness to design, build and deploy Business Information Systems.Technical skills· An appreciation of data warehouse design (e.g. dimensional modeling)· knowledge of C# and Web API’s would be beneficial· Familiarity with BI technologies (e.g. Microsoft Power BI, Azure Analysis Services, Tabular Models/DAX)Personal Characteristics· Proven abilities to take initiative and be innovative· Analytical mind with a problem-solving aptitude· Committed to excellence and capable of making tough decisions where necessary· Experience of planning, managing and effectively executing complex projectsThis is currently a hybrid home and office based role with a minimum of 2 days in the Kortext Bournemouth office, this may be subject to change.Job Types: Full-time, PermanentSalary: £24,000.00-£27,000.00 per year</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0B4I0z8Vg4C22bXJk453pUE2nnLCUOyY_R-ihB16RDW65dAXO9w17QY8SOm2HP94HqIyiNA8KaShSf6dwMd8CjUu6RxKxZaO118H6H1vWNfYPVDJ8LaTQMcUeB7_gLkOck5nLPsEPWfOW538iyOyMgSJcZDH_Vm83mG72CpqrWi_Yp7OKsiuodxtDiAeLvZqC2PLLFl9I4EuDh-XqZnAyAMggPlQU6iOjQx04jBQuttPrNJK1kiVLjdDLLZzpgv9OH3q_b4LqnMC7aT_v727om8wApaeXwpxJHkuvYCePm-xtF8JdZC12BM9gEa_3v0GHsEYodtr593JcRyKAQDDzkXTU_XhAYoaKGjqfsU7-hbe7mokqnovfZZxNTMzokq2QjJfQNvLY7ms3aRWN4hdUXpfJzOGBE_T6kg0uoq6GxTKPMxKcOo-crKCm1AvnuO0zxO1rIKJGpUrUEY9EledQcvnaFM2BFVMDUtuWSo7Mxsg3PuGccu1smYzE7X_Hn-o8KYwJs8D7u572MJNvSHhqFzkKbyAnIQDNZ3snrJ9zjCZOnW7H4wT3KaRKl9haxbYlXo_8fY3LnGkCYRv8tcjHyHvAXSoHLYIMAI_YHLxWywmEMLIaCGasnNSl8KIhpRF2xdwZFt7AetgDgJeU8NzafjEeqlofRveztbohgqGLqDSdPewRrOKSUV&amp;p=3&amp;fvj=0&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0ATA-436Np_sDHyRyXgfnC7rulQh_HAeSRkBVkE7CpmFpvNpKLrqjOCKBv_cBjIQcIzFdoU-nk55maFpcPaQtuCK3Pu9nBlhvXd7Ce7kPpIfroWykSyCGN9KAvjnfkDWzaHeu1WqngiHkACAmYTjTsEGXos1QpYSfe15u5XqPr7OTudoUcZqTqUCvnBwF_Yd10bdiD8C1EYIh80AyQNSPo47smDhdv53TwIWLWGAyF3m2JOaJ6NxiI6yQLyjIhHnVGrkQdFFMsweLcb1JKo6Dv8GVto4MMZ6AB398uEznuc_Q796o_9ZLXdEDAc4D5Qrs-h9gzrKR0Kyy8OEl3ph9EcFx8Z0Ga7Fi6eGWPdvwDbMASvNkZQnWBZXmjWLdNypH0Yq6THS33HbwsZkjN58pYhjE6WYenq06QLllQR2eg6o2FZy205I96tosksKAnPCdrtzAW-wHNU7HDleynpKrKJKESkIIyMz_bFbAS5KYMWZg==&amp;p=3&amp;fvj=1&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -785,17 +687,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Data Analyst</t>
+          <t>Data and Insight Manager</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NES Fircroft</t>
+          <t>ODM Ltd</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>England•Remote</t>
+          <t>Southampton•Remote</t>
         </is>
       </c>
       <c r="E6" t="b">
@@ -803,66 +705,32 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Contract</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+          <t>£25,000 - £30,000 a year -  Full-time, Permanent</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>53.0444</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0:49:46</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Champions data quality across systems and leads periodic data reviews and data optimization.
-Participant in data governance committees.</t>
+          <t>Developing review processes to ensure data integrity is maintained.
+At least 2 years’ experience in a data / insight role.
+Job Types: Full-time, Permanent.</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Data Analyst - 12 Months Contract – Remote
-Essential: - Proficient in existing digital tools and processes (e.g. Power Automate). Experience in small to medium scale digital projects. A working knowledge of software programming. Experience in data mining and analysing. Understanding of machine-learning and operations research. Experience using business intelligence tools and data frameworks. Data Modelling to create Algorithms and predictive models.
-JOB SUMMARY
-The Data Analyst is responsible for addressing critical data-related business problems by creating strategies, to analyse, connect and draw conclusions from clients systems, data lakes and external sources using robust data science techniques. Working with Business subject matter experts, the role will be familiar with labelling standards and compliance measures and will play a key role in supporting portfolio decision making and process development.
-The Data Analyst is also a critical contributor to discussions around data architecture and standards led by Information Management (IM) and Digital.
-The Data Analyst interprets and analyses data to provide innovative solutions to problems, designs data modelling processes to create algorithms and predictive models or performs custom analysis as required. The Data Analyst will support and/or lead initiatives relating to machine learning and artificial intelligence, representing GRA in discussions with Information Management and Digital.
-The Data Analyst will be responsible for effective compliance monitoring and support time-critical provision of analysis of labelling data.
-The role also acts as a key interface with IM providing SME for system requirements and data quality. In addition, you will be expected to lead or participate in imitative to improve efficiencies.
-JOB RESPONSIBILITIES
-Proactively identify and extract valuable data from multiple sources and automate collection processes
-Participant in data governance committees
-Undertake pre-processing of structured and unstructured data
-Sift and analyse data from multiple angles, looking for trends that highlight problems or opportunities
-Builds and implements predictive models and machine-learning algorithms
-Use a combined knowledge of computer science and applications, modelling, statistics, analytics and maths to solve problems
-Maintain effective relationships with other platform lines and Business Units enabling facilitation of effective portfolio delivery
-Present information using data visualization techniques
-Become a subject matter expert in 1-2 digital. Automation skillsets (e.g. functionality mapping, predictive analysis)
-Create awareness by working across functions to share and learn about best practices.
-Lead or participate in ILG and or GRO technology initiatives
-Developing best suited data models and algorithms in collaboration with Information Management and Digital partners
-Assessing the effectiveness of the data model with the ability to select the right technique of data gathering.
-Champions data quality across systems and leads periodic data reviews and data optimization
-Point of contact for labelling compliance data.
-Takes appropriate risks to advance new concepts and methodologies for the design and optimization of data analytic projects.
-Use modelling to create the optimized customer experience.
-QUALIFICATIONS / SKILLS
-Proven experience as a Data Analyst or Data Scientist
-Proficient in existing digital tools and processes (e.g. Power Automate)
-Connective thinker, able to challenge and suggest optimization through data and insights.
-Experience in small to medium scale digital projects.
-A working knowledge of software programming
-Experience in data mining and analysing
-Understanding of machine-learning and operations research
-Experience using business intelligence tools and data frameworks
-Analytical mind and business acumen
-Strong math skills (e.g. statistics, algebra)
-Problem-solving aptitude
-Ability to be flexible, adapt to change work independently, as well as part of a team in a matrix environment.
-BSc/BA in Computer Science, or relevant field; graduate degree in Data Science or another quantitative field is preferred
-Candidates must be eligible to work in the UK
-With over 90 years' combined experience, NES Fircroft (NES) is proud to be the world's leading engineering staffing provider spanning the Oil &amp; Gas, Power &amp; Renewables, Infrastructure, Life Sciences, Mining, Automotive and Chemicals sectors worldwide.With more than 100 offices in 45 countries, we are able to provide our clients with the engineering and technical expertise they need, wherever and whenever it is needed. We offer contractors far more than a traditional recruitment service, supporting with everything from securing visas and work permits, to providing market-leading benefits packages and accommodation, ensuring they are safely and compliantly able to support our clients.</t>
+          <t>ODM are currently recruiting for a Data and Insight Manager to join our growing team. Due to the acquisition of new clients, we now have the requirement for a dedicated resource to support our clients and field sales team by creating, analysing and presenting data.In this role, you will work across multiple clients, producing reporting to each of their requirements. This varied role will require you to think about the longer-term development of our reporting ensuring we use the tools available to us to their full potential.You will be responsible for: · Developing our reporting systems to bring them in line with our future business development plans· Delivering accurate reporting, as per the agreed client specifications and timescales through Excel, Google Data Studio and Power BI· Using internal and third-party data sources to provide analysis on customer performance· Developing review processes to ensure data integrity is maintained· Questionnaire/survey creation and refinementThe ideal candidate: Proficient in MS Office - advanced in Excel and Access (Power BI knowledge is preferable)Strong mathematical and numerical skillsDetail oriented, an inquisitive mindset with solid problem-solving skillsExperience in presenting dataGood communication skills and ability to stay calm under pressureAt least 2 years’ experience in a data / insight roleWhat’s on offer?· Competitive basic salary of £25k - £30k depending on experience· Annual holiday allowance of 25 days plus Bank Holidays· Company pension scheme after 3-month probationMostly home working opportunities with some travel to our Winnersh, Reading office. Home/Office split discussion are available upon Interview.Now has never been a more exciting time to join ODM, we look forward to hearing from you.Reference ID: DIJob Types: Full-time, PermanentSalary: £25,000.00-£30,000.00 per yearBenefits:Company pensionOn-site parkingReferral programmeWork from homeSchedule:Monday to FridayWork remotely:Yes</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DiSGR40Z5TcCdl_J7A59VP_6ZDYIBt_zfNy0x5FbgpmDCyNykNdPc5kBSuTvSlweuLX7JnAe9oDhaM7icfTJ3MlVH4ryhWuJnpY1u7yEZY9DNdWvmFV2ydQfRpBFJWVpQCJYRLYFfeoufehI86UDd5kGewKnZ74pi1pthtszICjrdKwvJTb1zqtEgoIkq708TEt0e3VpVFGHuzCxmbEkDXZuFiQpwlmVe6_zlgT3QIoZLsTaQFmDxdFpC7zXsKBaKzrVsXNgEzjxty_3FdmIYVWeEVvYABZSDaB4fbRoVp3V7EunMPRAcXs5niGuXWFHRanU-DmpJilDbgsogLVCHmBQ1_4k4PppwNw9ot0f8WuqcLdP6INXFt64LWdvBz2lhLe4HB-qDmbVzt2iPaUMe0ZPdFz5B1nKINwOINNw-6Ok0-79qAmmBJNfeCPqQFlBKk1y1PugyJcSxuM7_4123LfxXQWCpANfGMpZgtb7gudXZJz8lSc_--91rMRhDJrWZ_0HJ0LHTjsOajnR0AmqeTr0xTzOSR0sTZu3ug-08XcQkri6oUuVJTU1Iz2m7FQvH_aCLe_7vUQ71Eukh8GeSePJU1YCTiZU4CYQ821lljFWD2V5q3xtLcFCnuqnSUTnQ=&amp;p=4&amp;fvj=0&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DME5u13oovQFoCdjnUW-hiHsOb3xRhlrCPVAit2xJY4ba4NQNlnLcuSLydemmEEtR5h-gTrOkKB01xRlLAylBRt4ZtVPI4mCIIdoHlP_WofL7PyFiOgvSGHDKv_EZd0kgdJX7vwD20GW4LJIVXLlcW5bm4fZmfc0NmBM1ADigTPQTfSRmFiB21uCxgqfl6idZIyUdiXJ5Wv3QArT7iAVguK6Z87riFArTRq35LWOSPzzLdG0HtMOTUbmHh-HfJBUuV16eFN_pl399xxIdNmqWsV7Lkl2w3eZqn2Ppc8sTDFQEuHiOU0yd68eAgYG3w7-76HekhNj1X4vtKFe64bgN4Sc32qNYdUi1-Zcec50RzPYthq48HUPF0Yg6T4g3PsRhuwOyZbSjpZXhDEBV31nRCBv6IJVANGqp-BVbdvzlcnDvq-bkYvGhWby5SV_Vyzl92l-ch5I5zULZ8smmVRdINHIhxm7TZKsD-Yr_-b-V_ew==&amp;p=4&amp;fvj=1&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -872,74 +740,49 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Product Manager - Unity Platform: Intelligence &amp; Analytics</t>
+          <t>Email Marketing Specialist</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>JPMorgan Chase Bank, N.A.</t>
+          <t>Runderwear™</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Bournemouth</t>
+          <t>Poole BH14 9EX</t>
         </is>
       </c>
       <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>£24,000 - £26,000 a year -  Full-time, Permanent</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Full-time, Permanent</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>9.039200000000001</v>
-      </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0:14:30</t>
+          <t>0:00:00</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Conducting research and providing ideas on using Unity data to develop analytics to identify process improvements and new client opportunities.</t>
+          <t>Segment audiences based on predefined attributes and demographic data.
+Analyse data and metrics for individual campaigns with an attitude of continual…</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Department and program description
-The Interaction Management Program consists of a portfolio of initiatives aimed at transforming and delivering better ways of working for DPS Operations when they interact with each other and with their clients. The Interaction Management team is a dedicated group of Product and Program managers focused on managing a broad product portfolio, including daily operational support of existing products, and initiatives that support the transformation of the operational landscape. As a team we are focused on outcomes, being data driven, learning through experimentation, and collaboration with cross functional teams including Technology, User Experience Researchers &amp; Designers, Data Science, Product Marketing and Operations.
-The Interactions Management team aims to improve the Operations user experience through the design, development and delivery of a suite of capabilities that leverage new technologies to address operational needs when managing the resolution of exceptions and enquiries. Delivery of these capabilities will empower users to make process changes, enhance controls, create resource capacity, enable better analytics, and improve the user and client experience.
-Unity will be the CIB cross-LOB enquiry and exception case management platform removing the need for LOBs to build separate case management systems. Unity will be an open platform, allowing LOBs to connect to it in the manner that suits them best.
-Role description
-The successful applicant will be part of a global product team responsible for the delivery of Unity - the new cross-CIB case management platform to be used initially by CIB Operations. The individual will support with the delivery of Unity intelligence and analytics capabilities, partnering closely with the Unity Product Managers, Technology, User Experience Researchers &amp; Designers, Data Science and Operations teams. Responsibilities include:
-Participating in the delivery of the Unity Intelligence &amp; Analytics product roadmap; from ideation to setting priorities for planning and execution
-Identifying business needs, detailing business requirements, and partnering with Design,Technology and Data Science teams to deliver the product capabilities
-Applying agile methodologies (i.e. writing EPICs user stories etc.) highlighting the value delivered by each requirement and release
-Conducting research and providing ideas on using Unity data to develop analytics to identify process improvements and new client opportunities
-Contributing to the user outreach strategy &amp; rollout in partnership with client service teams
-Building and maintaining relationships with stakeholder groups, and promoting the Unity brand and product
-Work across global Risk, Legal and Compliance organizations to ensure functionality is fully compliant with all regulatory and data privacy requirements
-Required skills and qualifications
-Prior experience of Product Management in financial services
-Experience managing strategic product development and process re-engineering initiatives
-Prior experience and understanding of CIB Operations business areas and trade lifecycle knowledge preferred
-Ability to build solid relationships within a short time period
-Excellent communication skills
-Structured approach to problem solving, and decision-making
-Attention to detail, seek out potential problem area, conduct root cause assessment and synthesize findings to formulate recommendations
-Prioritisation and organisational skills
-Ability to work under pressure to meet deadlines
-Curious, inquisitive and motivated to deliver value to users &amp; clients
-This role provides an excellent platform to be involved in the transformation agenda across the CIB, D&amp;PS and LOBs.
-J.P. Morgan is a global leader in financial services, providing strategic advice and products to the world's most prominent corporations, governments, wealthy individuals and institutional investors. Our first-class business in a first-class way approach to serving clients drives everything we do. We strive to build trusted, long-term partnerships to help our clients achieve their business objectives.
-We recognize that our people are our strength and the diverse talents they bring to our global workforce are directly linked to our success. We are an equal opportunity employer and place a high value on diversity and inclusion at our company. We do not discriminate on the basis of any protected attribute, including race, religion, color, national origin, gender, sexual orientation, gender identity, gender expression, age, marital or veteran status, pregnancy or disability, or any other basis protected under applicable law. In accordance with applicable law, we make reasonable accommodations for applicants' and employees' religious practices and beliefs, as well as any mental health or physical disability needs.</t>
+          <t>Company descriptionThe Runderwear story began as a solution to a problem that is the bane of many runner’s lives - chafing.Runderwear’s founders, Jamie and Richard met at Loughborough University when they were put in the same corridor in Halls of Residence and instantly became friends. Both shared an incredible enthusiasm for sport and Richard was a track and cross-country runner whilst Jamie played most sports, particularly football.After university Jamie started to run more and decided to do the New York Marathon. Whilst there, he realised that whilst he had great technical outer clothing, he was wearing his usual underwear which was chafing. Jamie searched the New York Marathon expo for some performance underwear, but all he could find was a pair of large Women’s Hot Pants! Not ideal!On Jamie’s return to the UK, he and Richard started to look for good running underwear; they tried a few brands, but nothing was right, so they decided to make their own and Runderwear was born!Fast forward to winning ‘Best Underwear &amp; Socks Brand’ for three years in a row at the 2018, 2019 and 2020 Running Awards. The Runderwear range has grown to include different styles of performance underwear, running bras, socks and base layers.As the Runderwear product range expands, Runderwear’s dedicated ethos remains focused on creating chafe-free comfort for runners.Job descriptionRunderwear is looking to recruit an Email Marketing Specialist to help evolve our email marketing and take it to the next level. The business is seeing rapid growth and see the email channel as a vitally important customer communication and engagement opportunity.The Email Marketing Specialist will be given the chance to really shine in this fast paced and energetic environment, a chance to really expand their digital abilities and grow with the team. This is a great opportunity for someone with 2+ years experience to take the next step in their career.You will be pivotal to the delivery of our email marketing strategy to our customers, creating both campaign and triggered flow emails. From campaign concept through to campaign analysis you will be able to take ownership of the email channel within the business. For the UK market the role would be looking to build upon a solid foundation of campaigns and introduce innovation and regular testing to optimise performance. For our US and Australian markets there’s the opportunity to create a campaign plan in partnership with the country managers and marketing team. You will introduce a consistent look and feel to our email communications across all of our markets and across our campaign, flow and transactional email marketing.RequirementsBuild creative and engaging content for campaigns using the Klaviyo email solutionSupport email campaigns by developing content marketing strategies and technical enhancementsDrive email strategy and campaign planning by analysing performance and KPIsIntroduce best practices for list management and deliverabilityAnalyse data and metrics for individual campaigns with an attitude of continual improvementProvide recommendations for new and existing campaigns including flows, and other campaign triggers automationCreate A/B tests for campaign optimisation on many devices and platformsMonitor email list health and segmentation strategySegment audiences based on predefined attributes and demographic dataMeasure results and optimise lead nurturing email flowsProvide solutions to email marketing questions and concernsAssist the digital and marketing team with other marketing tasks like lead generation, product management, social media and analyticsAssist the digital team with website edits, sales reporting and customer enquiries.2-3 years of email marketing experience within a brand or agency.Good knowledge of email marketing trends and innovation.An excellent communicator with great organisational skills, with the ability to work to tight deadlines.Experience of working with active, sports brands would be an advantage.Personal SkillsPassionate about your work and have an excellent attention to detail.Good verbal and communication skills.Good time management.Self-motivated with a sense of ownership.A passionate creative designer who enjoys developing ideas.Happy to work from home and ability to collaborate remotely.Agile and copes well under pressure.A friendly, open, honest team player.Job Types: Full-time, PermanentSalary: £24,000.00-£26,000.00 per yearBenefits:Additional leaveCasual dressCompany eventsEmployee discountFlexible scheduleSick payStore discountsWork from homeSchedule:Monday to FridayEducation:A-Level or equivalent (preferred)Experience:Marketing: 1 year (preferred)Work remotely:No</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/rc/clk?jk=36447c0457e010f9&amp;fccid=aaf3b433897ea465&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0Abv5PlfV47PFnF1a4rIT5lO8wuZZhQ0hqSSN5OCEN_ajLNwcd0IyxorlwP3q6gyaMqFCPP3ejhN0KVnYtyp_TNgs2ZOyWUt6-p_n_0jnjVKWvmw2eR4Xr-0WdtPdK5XJiCljJRudPbhNjc9evAltjtGM6qVNG7Sk-n87Z3705Uhx3bzUV6irGVt2zDYyYlkoJoBjlRthOH0tITaXzkTN0HzCkcvvIvGtVR4GwI81OW0BelmVe4TpqrAQAVanD6qR-kVGgoSP1JD0fimv9H7JRpTXWd-j606N__I7eirx0EuEufSj2DLdTyuqR_tL80QEI5wDCi-_Ic2UcRtRXd_lXYqQf7PBi9GCbybHiknprRXx-IZj6u9AMMR6BMZ8IZ_hl0FzIPW3nb7Fcagy3JIfOwrEkv5u9CFlwPK-V7lz38aXlIDh-_2E3XD2ev-I8xeMMxpC0xL1tRXRw_l6iC2y7_AVq9IMsmfqM=&amp;p=5&amp;fvj=1&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -949,75 +792,530 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CIB - Interaction Management - Unity Reporting &amp; Analytics P...</t>
+          <t>Office Administrator</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>JPMorgan Chase Bank, N.A.</t>
+          <t>South Coast Windows</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>Poole BH15 3SS</t>
+        </is>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>£10 - £12 an hour -  Full-time, Temporary</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Performing data entry roles, including updating records and databases for personnel, financial and legal information.
+Monday to Friday 8am to 4pm (1 hr lunch).</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>SCW Ltd. is a private Window and Door installation company specialising in UPVC and Aluminium products. We enjoy a solid reputation with our commercial and retail customers, offering a first-class service to the south and southwest. We are looking to grow the business to the next level after completing several high-profile jobs. We are looking for a highly organised and communicative Administration Assistant to bring some essential organisation skills to the team.Managing the reception, including welcoming customers and guestsManaging company correspondence, including phone calls, emails, letters, and packagesHandling bookkeeping, budgeting, and billing cycles for the businessOrganising meetings and scheduling appointmentsPerforming data entry roles, including updating records and databases for personnel, financial and legal informationManaging inventory of office supplies, including stationery and multimedia equipment to ensure smooth office operationsCreating travel itineraries for all SCW employees working away.Maintaining a social media voice for the company on numerous channelsRecord staff and subcontractors’ absence and holidayEssential CriteriaPresentation skills and customer services knowledgeExceptional organisational and time management skillsOutstanding verbal and written communication skillsBasic knowledge of accounting procedures such as bookkeeping and other general financial proceduresProven experience in a related role such as Office Assistant, Receptionist, or other relevant positionKnowledge of computer programs used in daily office administration functions such as Word, Excel, CRM, and Project Management Software.Proficiency in filing and paper management, including the ability to manage business correspondence and the ability to handle confidential informationExcellent problem-solving skills, the ability to research and an aptitude for helping other peopleMonday to Friday 8am to 4pm (1 hr lunch)Paid Monthly£10ph to £12ph depending on experience - Casual Contract (reviewed after 3 months, full time may be available after qualifying period)Reference ID: ADMIN-SCWContract length: 3 monthsApplication deadline: 16/09/2021Job Types: Full-time, TemporarySalary: £10.00-£12.00 per hourBenefits:Employee discountOn-site parkingSchedule:8 hour shiftMonday to FridayAbility to commute/relocate:Poole BH15 3SS: reliably commute or plan to relocate before starting work (required)Experience:Administrational: 1 year (required)</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0Cf301rU0dGBi37IMLhu2cgLU5eNeoSgKTwu1xoBEa4CWIvtoks4OFnBrD4fPfiEUizI0c5PJj6OOSve8lsykqUJZQbpo3yvKEHpU9C_rL6rMlDIWEbUOnkNYUC6oPYm4_Ow_whm6TdhnrgJSTJnYRxLc36riMZ4DgCqm3GV64doXMIu96TYPJgyuuU6f6Zhy619H_Q-Lgoqm7ku-RvnHYapOhHyjNjg-7Rt1UgJETpsBtdBzFdZLhpLUHSyuuACEvHFlklcZhQsCom9LHFRn8yh4XjIpBw3iaLJS4XxLrdb5nTH3v8XtsLnHQsE-03D88SxgPSGjqBNNrymlAUM7Bi6iEyBlsThTmDS7J9Wlg6nXc7RAVX_gE9k4LgWTCoUb7A1RIEYluXCCBvaljW8IdTOpcmlPC8-J5JK-hOzp9hfCdIKjiAmnVDjb_kHppTxxvO90k5sGfgaB5pV8SDKL7p&amp;p=6&amp;fvj=1&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Administrator/Credit Controller</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Wessex Glazing and Building</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Bournemouth BH9 1LT</t>
+        </is>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>£10 - £12 an hour -  Full-time, Part-time, Permanent</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>9.039200000000001</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0:14:30</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Administration tasks such as - data entry in an accurate manner, updating records, reviewing documents.
+Previous experience is desirable and organisational…</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>About usWessex Building ContractorsWe are seeking a new individual to join our growing team in a good working environment to carry out administrative, credit control and general book keeping input duties. We are looking for someone to join us long term and that works well as part of a team.Previous experience is desirable and organisational skills are a mustThe successful applicants duties will consist of some of the following;Administration tasks such as - data entry in an accurate manner, updating records, reviewing documentsHandling email enquiriesCredit controlBookkeeping dutiesLiaising with customersAnswering telephonesThis role dependant on the applicant is negotiable as to part/ full time with some negotiation on hours.Part-time hours: 20-40 per weekJob Types: Full-time, Part-time, PermanentSalary: £10.00-£12.00 per hourSchedule:Day shiftNo weekendsExperience:Administrative experience: 1 year (preferred)Work remotely:No</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CsFP-xDvV-IXN_aFa68_SC2Ew9lsdfIsiVW_QF4AkFEfdjJHfBk_3lNImCqX0T1WMfKz1rLthjvZUcF7y7o8xsx1qDYQmC_r8_fC1Tsa33p2LRUxZ8qp6RZa8HH8UBh9RXimXweG_sB7fHnxH0LQtxqWB-PoEylXRq4jgsXM3ZsnKPYtcTjlt47KC7P67bjaa0WGMAPw9oPzyWYCQxMSEfWPZPIzYP8Xel9BKzIl1xutC-k3uBjJtNX0SdDHN_uy7kzWS7KXK7Dh-k-G3ive2XqMjBaJ5cB7e7d8ePDdTzYNbE6wFWjJDic4nXBTephiISnd2qMOxlUX08cXUpA1x1hXLCG-B0U7VpXK8Im_dA8gnrHoIEjBRm236pYWDGTjvIPINyTwJWAT-SQmVG5VNOsNxRN7oWX7w02hDvnDQtduvp9kGTUC_vC-fJ6EAcLK4ffdgZTr8Cv4onIsqSHuWXan64mHRg3uQ1j1sAMJwAwQ==&amp;p=7&amp;fvj=1&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Administrator / Credit control</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Wessex Glazing and Building</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Bournemouth BH9 1LT</t>
+        </is>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Part-time</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>9.039200000000001</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0:14:30</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Administration tasks such as - data entry in an accurate manner, updating records, reviewing documents.
+Previous experience is desirable and organisational…</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Wessex Building ContractorsWe are seeking a new individual to join our growing team in a good working environment to carry out administrative, credit control and general book keeping input duties. We are looking for someone to join us long term and that works well as part of a team.Previous experience is desirable and organisational skills are a mustThe successful applicants duties will consist of some of the following;Administration tasks such as - data entry in an accurate manner, updating records, reviewing documentsHandling email enquiriesCredit controlBookkeeping dutiesLiaising with customersAnswering telephonesThis role dependant on the applicant is negotiable as to part/ full time with some negotiation on hours.Part-time hours: 20-40 per weekJob Type: Part-timeSalary: £10.00-£12.00 per yearWork remotely:No</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CsFP-xDvV-IXN_aFa68_SC2Ew9lsdfIsiVW_QF4AkFERKxwh0C2TdbUcAwt3Hz19Jyt0ZYJJFvyIUGle9J6gQvPhjatUv0KHMi7QtYW_a21T4UCntEqr3MoyP8vE5_mmCVpwT8g_PkacPKiHj6oHMwDlPcrcKmX8MevfWihMHrb0Hy9qqsMRZYQAp7o0ZKzBH_y3a1DMFmB-6UJZIBoC_6ex7AU8pez447wBVRKXheEIdavGygXcbbV_YYu4nPlvV3xpfrARJKd9cM821HoQzY3o91wxjCZXd2h-DB_Ul5ludr78Tu3_7SqkIgcFKqud1NlNZLdl6EAzqHl1VElJLTEk7MQ3F1E1vUsVTPVVmvA9WWNA4EjRho_HVBnxi0dfoxAIUP6xXekpdjC1U7u0-WmGB2-Tb2wgOQhUVCH-JefqpWvXCnyEME18ZXdUofnsBtwqgWOw_Z_8FY3vuMZXqauwB8XtZKlgI=&amp;p=8&amp;fvj=1&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Data Insight Executive</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Buyingtime Limited</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Winchester•Temporarily Remote</t>
+        </is>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Full-time, Permanent</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Managing the delivery of the data needed to support the campaign team function, campaign data according to each project brief.
+Job Types: Full-time, Permanent.</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>The Data Detective will be responsible for providing support to the Campaigns team. The Campaigns team deliver market leading services on behalf of software vendors and specialist consultancies. This is only made possible through the creation of great data sets. The data detective is responsible for ensuring that accurate data and insight is made available to the team, in order for them to deliver great opportunities to clients. They need to be focussed, well organized, curious and proactive with an amazing attention to detail, whilst using initiative to find new ways or working and delivering continual improvement.The role involves building accurate and compliant data that includes, but not limited to, company contracts, business intelligence and insight. Once built, the data needs to be verified, often through telephone calls to businesses and stored correctly within our CRM. The specialist also needs to be on hand for any ad hoc additions as the campaigns are running to ensure our execs always have access to the most accurate and current information.Duties and responsibilities: · Maintenance and updating for all prospect data, including cleaning, acquisition, de-duping and loading into relevant systems.· Managing the delivery of the data needed to support the campaign team function, campaign data according to each project brief.· Database maintenance, detection, enhancement and improvement as required, identify ongoing activities to ensure success of the business generally, and enhancements required to support delivery of specific development projects.· Maintenance of all database records and actions required to ensure database integrity.· Verification of data through various methods, Linkedin, Companies House, verification calling etc· Delivering and promoting internal practices and making suggestions on process improvements and SLA’s.Qualifications: Highly PC literate in MS Office – particularly Excel.Experience with CRM systems (Salesforce), database management, maintenance and manipulation.Excellent internal and external communication skills.Reference ID: DDJob Types: Full-time, PermanentBenefits:Flexible scheduleOn-site parkingWork from homeSchedule:Monday to FridayExperience:database: 1 year (Preferred)Education:GCSE or equivalent (Preferred)Work remotely:Temporarily due to COVID-19</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0BXlCRMKhI-0nfndyxsvN-0LW9gcj768jP6b4uh4-yGNJ5PbIoGZVUzoZZhtpfYAgB3dnuEQnxRsd-KkR2Ql04LKX0yCFYXb-xh9mMB4C-o6SEsFus0QnibSdTDez320iEaJAKE5ffndUsvlOKtpBRyxv9sAr129VPqLv68bPisfq36jasprzQOkkXe0yzsZGAWrl-Qct-xfLuNIoTQPy2Bb0-KD0-6sRUMHfusLvR8KKjO0VRgfV66IZ1JqU-1AbujFCqmTARsPpqESPxXMSbykxowcP374smT9HjKazADbfruo-bnd4vX6ba6OqVzwcZ333j5nA5tGMq7fgZKBbJjrD5eyNKdP2b-FWsq2XoF8x20MQTF8OJ6T8Ab92BhjhEDGXX7XZyR7-l1Fes5j-9_nTaVijqmV8b8_9leE6VyYMGR2esFDiafHPIS3MDotr7_uSUk-rNV_TzUVF9g1zga2Q-WdHrkoi0=&amp;p=9&amp;fvj=1&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Screening Administrator</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Allied Universal (Europe) Limited</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Bournemouth BH7</t>
+        </is>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>£20,000 a year</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>8.325200000000001</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0:13:39</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Generating reports and analysing data using excel.
+Accurately document and enter data information into business systems.
+Salary £20,000 per annum..</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Are you hungry for a challenge?Do you have professional Screening Administrator experience?We are now recruiting an experienced Workforce Screening Administrator to join our Client’s team working in an established global investment banking firm in Bournemouth.As our Workforce Screening Administrator, you will be working in a fast-paced office environment, supporting all aspects of the screening process for the organisation’s prospective and current employees. You should have strong analytical skills, data entry and general administration experience.The ideal candidate is customer focussed with a professional outlook and possesses excellent written and verbal communication skills. The role requires the candidate to work independently and in the team; to multitask and to offer new solutions to procedures where appropriate.What You Get: Salary £20,000 per annum.Full time contract working Monday to Friday, 37.5 Hours per week. (Flexibility).Fast paced and exciting role, no two days are ever the same!Opportunity to work within a globally established Investment Banking firm, with the prospect to make a difference in a position of real responsibility.Duration of contract: Temporary 3-month contract.Core Duties &amp; Responsibilities: Accurately document and enter data information into business systems.Investigating and checking reports for further action.Liaising with other team members and team leaders to resolve queries and/or establish processes.Requesting additional information and checking emails for responses.Generating reports and analysing data using excel.To be considered for this excellent opportunity you must have the following: Proven experience of working in a customer facing role.Strong IT skills with solid experience of using Microsoft Office, Excel, PowerPoint &amp; Outlook.Ability to multi-task, prioritise tasks and work to deadlines.Ability to work in a fast based and pressured environment.Ability to maintain confidentiality and professionalism at all times.Commitment to deliver to exceptional standards.Ability to problem solve, pro-active and able to offer new solutions where appropriate.Please only apply if you are available and interested in a temporary 3-month contract.To apply, please forward a detailed CV and covering letter explaining your suitability for this role.A.U Recruit is an equal opportunity employer.Reference ID: SCRADMINJob Type: Full-timeSalary: £20,000.00 per yearSchedule:Monday to FridayExperience:Customer Facing: 1 year (required)Microsoft Office, Excel, PowerPoint &amp; Outlook: 1 year (required)Screening: 1 year (required)Work remotely:No</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DjrH4G27sm0BFXBS9q2tnCePsQHyNbDH0dm6ng2FAe5orHuuTmREBGDVTnoLV1LbFt-pUen5HA01EhN4T1oeQi-821SF2jtDSOdlQowFCFDNRAk6kM5nVRfxnFjfbmMfu_JJTce70gl5YFYwgaX9h9iXQerY7J5L2eRnPXaHDq49-6h68Hu1xXuc_Mb-Mx3ydXCyv4zlZgrJd8s8dbT16v7qLkugWa0cvbcmMZ5bokLipRzm9q4ezmYkTI3ycVy9kQ61Chdp-Kq09W0oDYFTJ3HP83I0AfQu9GoYkB-eMqIrt-zRO7D2j2zbbSumAlBBsz7l8jC4MK3qPQ3ag0m56__TXxhG0rl09nsFptC9587tH8Gp6SiSmljRFjr7_p6CCIXBJtgqpOU0dmJ-hi4KznHLkehF4kL701QzNQckwZ2yEvCkbfGvWVVV9Jth9DUtsO3JEEWFDuU4I6bLcInUQa7xDQaHrv8cY=&amp;p=10&amp;fvj=1&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Data Verification Administrator - 20th September Start Date</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Lead Forensics</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Portsmouth</t>
+        </is>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>£18,533 a year</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>82.9636</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1:11:30</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Previous experience in a data entry or inputting role would be an advantage but, isn't essential.
+Starting salary £18,532.80 plus, monthly bonus of up to £220.</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Data Verification Administrator
+Starting salary £18,532.80 plus, monthly bonus of up to £220
+Portsmouth, UK
+Summary
+Lead Forensics are one of the fastest growing software companies in the world. We can identify other businesses who have been visiting our client's websites and help them convert these passive visitors into actionable leads. We know that every business-to-business organisation can benefit from the leads our product generates.
+The Data Verification team focus on ensuring the Business Data we hold is accurate and provides a high level of information including website links, office locations and key contact information. Due to the success and growth of Lead Forensics we concentrate on adding new Business Data on daily basis to grow our internal databases.
+Due to growth across the Lead Forensics group we are now looking for highly motivated individuals who are looking for an opportunity to either move into or grow within a data focused career. We will offer full training and support so, prior experience within this industry is not a requirement.
+A little about the role:
+Conducting research to capture vital business information
+Capturing this information and accurately inputting into our CRM system
+Working to set processes with a high attention to the detail
+Working towards fixed targets with a flexible approach
+A little about you:
+Previous experience in a data entry or inputting role would be an advantage but, isn't essential
+High attention to detail and being able to work accurately with comprehensive processes is essential to success
+Computer literate with the willingness to learn new programmes and processes
+Ability to work towards pre-set targets or goals in a professional setting
+Desire to develop professionally and grow across our organisation
+Comfortable working on solo focuses but, still contributing in a team setting
+Why Lead Forensics?
+Receive a competitive base salary of £18,532.80 plus a monthly bonus of up to £220 directly linked to your own performance in role
+Opportunity to progress within a data career, receiving first class training and support to advance through the business
+Take some time out with our attractive holiday policy; start off with 20 days plus BH, increasing with each year of service (capped at 24)
+Birthdays off! (it's the most important day of the year!)
+Give back to the wider community with 2.5 paid Charity days, volunteer days, fundraisers, charity events
+Receive benefits such as the Employee Assistance Programme, sick pay, maternity/paternity pay, free on-site parking, free on-site gym
+When we are all back together again, company socials, Regatta, Family Fun day, subsidised Ski trip, Christmas parties
+What happens next?
+Simply apply and someone from our recruitment team will be in touch.
+Due to a high volume of applications we are unable to reply to individual applications specifically</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CwEYGYm6infS5AhLLwQ8WEatQRFkyqKWfaCmrQZb9b_XrMB6WPt1kgpShhHaazfah9L4GjL2OkH-nNrZJ8sLr0bVKjIF8h2uI95xKkY70ycPazIRBP_xvB9_VbxYrEeRvjA4PljPv94vd3_QkunPHDClGXcJa69iDM9KIXnjxj6qrMwwYUqvUU3p3h-70azM_TeKreOtImGaOxmTTORipTdNHmL86GwRv7K0kbkA0fAWG6ZLYI38eTlzqTYJysF-6Ps3Ow7iHdYOdHoV1HjDGCCOxoDqzdcmGZgKqAexq8E4-9rgyj2LUqj4qFf1rQkKJKG40H0d0yUAjO-N6dQoWlyehBNq3Uirs3ESPboOVr-rtMbXUkObkUij4HuCGlGMnThtUm-q1m94hoIcHyitylHcGooUwvg7AyfStik7xjkLaSelfqxLYbjNpa1GbDGdbizNx8cJL7lvHHrVnuV0hHwZQU4lx941MWHfLUCSl4xzbJaJ5zCGdFqL9Pr_G4HmyCkh3CxtrJmfRNLRBcGYiM0-Ex4OKk5-4=&amp;p=11&amp;fvj=0&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Data Support and Analyst</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Dorset HealthCare University NHS Foundation Trust</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Poole BH17 0RB</t>
+        </is>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>£25,655 - £31,534 a year</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>If you have the necessary knowledge of using and interpreting data, a flair for accuracy and attention to detail, numbers, patterns and trends plus a good…</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>The care our Trust delivers is rated as Outstanding . Within the Nursing, Therapies and Quality Directorate our drive is to support all our staff to continue the provision of high quality and safe patient focussed services. To do this we need accurate information and data to measure and monitor.
+If you have a passion for enquiry and to show where innovation results in improvement then this could be for you. The data support and analyst role will work closely with a large and varied team to understand what we need and how we can achieve it; Often to scheduled request but sometimes reactive.
+If you have the necessary knowledge of using and interpreting data, a flair for accuracy and attention to detail, numbers, patterns and trends plus a good natured approach to informing others then this could be the role for you.
+Excellent communication skills are a must as well as a sense of humour and flexible approach enabling you to engage with services.
+It is essential you are able to build and maintain excellent working relationships with stakeholders.</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/rc/clk?jk=d6f24b2aa3533e8b&amp;fccid=980c8c15a44d700b&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Temporary Administrator</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Rubicon People Partnership</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>Bournemouth</t>
         </is>
       </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Full-time, Permanent</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>£9.50 - £12.00 an hour -  Temporary</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
         <v>9.039200000000001</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>0:14:30</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>As a team we are focused on outcomes, being data driven, learning through experimentation, and collaboration with cross functional teams including Technology,…</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Department and program description
-The Interaction Management Program consists of a portfolio of initiatives aimed at transforming and delivering better ways of working for DPS Operations when they interact with each other and with their clients. The Interaction Management team is a dedicated group of Product and Program managers focused on managing a broad product portfolio, including daily operational support of existing products, and initiatives that support the transformation of the operational landscape. As a team we are focused on outcomes, being data driven, learning through experimentation, and collaboration with cross functional teams including Technology, User Experience Researchers &amp; Designers, Data Science, Product Marketing and Operations.
-The Interactions Management team aims to improve the Operations user experience through the design, development and delivery of a suite of capabilities that leverage new technologies to address operational needs when managing the resolution of exceptions and enquiries. Delivery of these capabilities will empower users to make process changes, enhance controls, create resource capacity, enable better analytics, and improve the user and client experience.
-Unity will be the CIB cross-LOB enquiry and exception case management platform removing the need for LOBs to build separate case management systems. Unity will be an open platform, allowing LOBs to connect to it in the manner that suits them best.
-Role description
-The successful applicant will be part of a global team responsible for the delivery of Unity - the new cross-CIB case management platform to be used initially by CIB Operations. The individual will manage the delivery of Unity reporting and analytics capabilities, partnering closely with the Unity Product Managers, Technology, User Experience Researchers &amp; Designers, and Operations teams. Responsibilities include:
-Defining key aspects of the product strategy and implementation phases; from ideation to setting priorities for planning and execution
-Driving the product roadmap, detailing business requirements and partnering with Design and Technology teams to deliver the product capabilities
-Applying agile methodologies (i.e. EPICs, user stories etc.) highlighting the value delivered by each requirement and release
-Conducting research and study on best in class reporting and analytics capabilities
-Contributing to the user outreach strategy &amp; rollout in partnership with client service teams
-Owning the OKRs for the Unity reporting and analytics
-Building and maintaining relationships with stakeholder groups, and promoting the Unity brand and product
-Responsible for a team of Unity reporting and analytics product owners
-Required skills and qualifications
-Prior experience of Product Management in financial services
-Experience managing strategic product development and process re-engineering initiatives
-Prior experience and understanding of CIB Operations business areas and trade lifecycle knowledge preferred
-Ability to build solid relationships within a short time period
-Excellent communication skills
-Structured approach to planning, problem solving, and decision-making
-Attention to detail, seek out potential problem area, conduct root cause assessment and synthesize findings to formulate recommendations
-Prioritisation and organisational skills
-Ability to work under pressure to meet deadlines
-Curious, inquisitive and motivated to deliver value to users &amp; clients
-This role provides an excellent platform to be involved in the transformation agenda across the CIB, D&amp;PS and LOBs.
-J.P. Morgan is a global leader in financial services, providing strategic advice and products to the world's most prominent corporations, governments, wealthy individuals and institutional investors. Our first-class business in a first-class way approach to serving clients drives everything we do. We strive to build trusted, long-term partnerships to help our clients achieve their business objectives.
-We recognize that our people are our strength and the diverse talents they bring to our global workforce are directly linked to our success. We are an equal opportunity employer and place a high value on diversity and inclusion at our company. We do not discriminate on the basis of any protected attribute, including race, religion, color, national origin, gender, sexual orientation, gender identity, gender expression, age, marital or veteran status, pregnancy or disability, or any other basis protected under applicable law. In accordance with applicable law, we make reasonable accommodations for applicants' and employees' religious practices and beliefs, as well as any mental health or physical disability needs.</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>https://uk.indeed.com/rc/clk?jk=710caae206b49a82&amp;fccid=aaf3b433897ea465&amp;vjs=3</t>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Temporary Administrator, Bournemouth, up to £12.00 per hour Are you immediately available and looking for the next step in your career? Well look no further,…</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Temporary Administrator, Bournemouth, up to £12.00 per hour
+Are you immediately available and looking for the next step in your career? Well look no further, Rubicon are recruiting for a variety of exciting office opportunities in the following departments:
+IT &amp; Technical
+Customer Service
+Administration
+Data Entry
+Marketing
+Finance &amp; Payroll
+Human Resources
+We have a number of temporary, with a view to permanent, Bournemouth-based vacancies paying between £9.50 - £12.00 per hour.
+These temporary-to-permanent opportunities are suitable for those with and without office experience, whether you're looking for your next job or wanting to gain knowledge in an office environment.
+Own mode of transport is preferred but not essential!
+If you're interested in hearing more about these positions, please apply below or call Maria on 01202 688 554.
+INDOFF</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0A9WFrdhlRjrF8LdCCgb1p4b_fTD3dePIFwz0VAmfbYR1YnmxRkLS3XvaKeOIupy86Ay5SO8FyJYV44xuvAgeWeCFmCZKOuc1uarJh_chYRZnuayK55ovGP-lAtQd-b7CnrLKGEOyuA4r0xJluFprIOay8ym7kO8uUgadSJYVY70ywF4X8i_JfidyigZ8bgsgzJFBOMPDJYCjszURhWtTWbMPGs2AT_guU8T8LriJzzPigAFpX2RLn7VnQ7-uVD1Zf8A0-Fjt1AYPK9OnhNheIQC9hZvFe_jC8sjVkD5i1MXCujFiNiQ_yYiXt7ojiKtnVtdiYzzSR4K2YoX-VJJ5PVw3FCA318qpAV-0O11qw2Kv9_l5axPzJQYYWp2rGJpax7vD6KOL1CjmIs1KiODF6_CMnAAvOlwTVBW4PBcvyv5ZoHdoxHRNhA_8p6XMjz4P0Qk7hnXR-U0To03IP4ys-qJtgwDkHGtyNsvxjWkd2GZIo59dcDvWkX1gDRil5GURr41CssRyyJDg==&amp;p=13&amp;fvj=0&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Data Analyst (Remediation)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>experisuk</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>England•Remote</t>
+        </is>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Contract</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>261.4277</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>3:09:11</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Reporting and data visualization skills.
+The Analyst will also identify and correct problems in our data sets, including performing quality assurance on…</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Job Title: Data Analyst (Remediation)
+Duration: September 2021- August 2022
+Work location: 100 % remote (work from home)
+***Umbrella Only***
+We are working with a well-known organisation, who are seeking for an additional Data Analyst to the team to provide support for security, innovation, and remediation efforts across the enterprise.
+As a Data Analyst you will collect, collate, analyse, and report on data from various data sources, internal teams, existing technology systems that span several technical and business domains.
+You will assist in translating operational data and information into actionable insights the team can utilise to secure the enterprise. Therefore, you must have good interpersonal communication skills, an analytic mindset, and is detailed-oriented.
+Required Technical and Professional Expertise:
+Basic knowledge in Programming / Scripting skills in languages such as SQL, Python and/or R, a plus
+An analytical mind and inclination for problem-solving
+Some experience with statistical software
+Knowledge of data gathering, cleaning, and transforming techniques
+Reporting and data visualization skills
+Basic understanding of data warehousing and ETL techniques, a plus
+Proficiency in Microsoft Excel
+Technical writing skills
+Excellent attention to detail
+Areas of Analytical Focus (with some basic knowledge and understanding of)
+Responsibilities:
+The Data Analyst will gather information from various sources and interpret patterns and trends to aid in data collection / analysis.
+Integrate and convert data into standardized format(s) for further analysis.
+The Analyst will also identify and correct problems in our data sets, including performing quality assurance on imported data.
+Evaluate information to reach conclusions, build models, test data set validations, and clean data sets to ensure accurate reporting.
+Define new data collection and analysis processes
+Basic understanding of data visualization and curation to present to technical and non-technical audiences alike
+Work with team members, management, and project stakeholders to prioritize business and information needs
+Look for opportunities to improve data collection and analysis processes</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0BqglzVP6e-OBouayVSRGNq4vL4YQ3xa44oZrpa481BKHcr7EIxusmGq7AYEJB4kEYg4k_YpVKsW0_qp0KGq5QYJq1VklYz5TRC5x0kIPUO6uHBp3a4k2kzz7tgL4fv-6gOI0SYbLLC9Cx2iRqEkfg_xqIJDcWEblmeO2SnCGyHFOD3X-isIEynkhFg7mjiwZ9JPYIiereLBiACHii3eqJ08M33PJJuBGqncCSMXsB4g6XJ2qfHwisJpO-vn3x3g-roHD1mz_VgV_WqnCZ37th7DLedko4hV39FmmDAd4C1D_QWlGd1Sd0KBNkgSHrhrQtV6fOKzccWK6_zPpKjdyJwQTHGpC1RM_VM7uYUxnp5ZwJmCNmiOQwzz7lJ9cgPDXjwkZvNum6ex2HJEruHdLTfEJmr3Fn8JV7cgZWLGB_v-zD4pHokSZSLPXsue0wCh0iLbOrTVzIrwKifR9-_JDcXhxoH_qTkDio74exym4UCJs3sUj9JmWtpNQNNElRey5sVsrde5maoKIzunQ0oqpO5&amp;p=14&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>

</xml_diff>